<commit_message>
feat : story, message데이터변환
</commit_message>
<xml_diff>
--- a/RawData/excel_files/DataTable.xlsx
+++ b/RawData/excel_files/DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grays\Desktop\Project\Unity\OIlNamProject\RawData\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E03906C-23DD-4FDA-9DCD-DFDDF741E052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B5CE41-108C-49B3-8C32-0DFCF3BFCE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31425" yWindow="975" windowWidth="20010" windowHeight="11385" activeTab="2" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
+    <workbookView xWindow="5625" yWindow="1275" windowWidth="20010" windowHeight="11385" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
   <si>
     <t>Name</t>
   </si>
@@ -96,27 +96,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>\n\n전 세계에 균열이 발생했다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>true</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>차원 간의 균열이 열리며\n튀어나온 온갖 마물들은\n그야말로 자연재해였다.</t>
-  </si>
-  <si>
-    <t>하지만,\n인류는 멸망하지 않았다.\n\n균열에서 새어 나오는 마나를 받아들여 특별한 힘을 지니게 된 사람들 덕분이었다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내가 바로 그 힘을 가진\n\n'헌터'다.</t>
-  </si>
-  <si>
-    <t>나는 협회에 소속된 헌터다.\n그것도....\n헌터에 관련된 계약에 허점이 많은 시절에 계약하여 노예와 다름 없는 계약...</t>
-  </si>
-  <si>
     <t>큰 계약금을 제시하여 계약금에 홀린 헌터들을 협회에 묶어놓은 다음, 거액의 빚을 지게 하는 계약.</t>
   </si>
   <si>
@@ -129,12 +112,6 @@
     <t>하지만 빚을 갚기 위해서라도 계속 일을 해야 한다.</t>
   </si>
   <si>
-    <t>(사이렌 소리)하… 또 균열이 발생했다.\n뭔 놈의 마물이 이렇게 하루가 멀다 하고 매일 나오는지 지겹다 지겨워…</t>
-  </si>
-  <si>
-    <t>(전화벨소리)왜?\n(중얼거리며) 아니...학교에서 필요한 준비물이 있는데..\n귀찮게 연락하지 말고, 카드로 사\n(뚝 끊음)\n</t>
-  </si>
-  <si>
     <t>하…귀찮네…</t>
   </si>
   <si>
@@ -142,19 +119,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>text</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delete</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -305,6 +274,34 @@
   </si>
   <si>
     <t>잘했다. 역시 날 닮았군</t>
+  </si>
+  <si>
+    <t>&amp;&amp;전 세계에 균열이 발생했다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>차원 간의 균열이 열리며&amp;튀어나온 온갖 마물들은&amp;그야말로 자연재해였다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하지만,&amp;인류는 멸망하지 않았다.&amp;&amp;균열에서 새어 나오는 마나를 받아들여 특별한 힘을 지니게 된 사람들 덕분이었다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내가 바로 그 힘을 가진&amp;'헌터'다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나는 협회에 소속된 헌터다.&amp;그것도....&amp;헌터에 관련된 계약에 허점이 많은 시절에 계약하여 노예와 다름 없는 계약...</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(사이렌 소리)하… 또 균열이 발생했다.&amp;뭔 놈의 마물이 이렇게 하루가 멀다 하고 매일 나오는지 지겹다 지겨워…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(전화벨소리)왜?&amp;(중얼거리며) 아니...학교에서 필요한 준비물이 있는데..&amp;귀찮게 연락하지 말고, 카드로 사&amp;(뚝 끊음)&amp;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -692,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8FABB6-B12D-4D0B-ADBA-E809D3A5F66E}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -704,24 +701,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -751,10 +748,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -762,10 +759,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -773,10 +770,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -784,10 +781,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -795,10 +792,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -806,10 +803,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -817,10 +814,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -828,10 +825,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -839,10 +836,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -850,10 +847,10 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -861,10 +858,10 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -872,7 +869,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>20</v>
@@ -905,7 +902,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -917,16 +914,16 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -957,7 +954,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -969,16 +966,16 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1004,7 +1001,7 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1030,7 +1027,7 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1056,7 +1053,7 @@
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1082,7 +1079,7 @@
         <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1108,7 +1105,7 @@
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1122,7 +1119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40025AE-C7D8-4357-9319-EFD6B75D65B3}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1138,22 +1135,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1161,7 +1158,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1170,7 +1167,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -1178,22 +1175,22 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1201,16 +1198,16 @@
         <v>3001</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D4" s="3">
         <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -1221,16 +1218,16 @@
         <v>3002</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D5" s="3">
         <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F5">
         <v>10</v>
@@ -1241,16 +1238,16 @@
         <v>3003</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D6" s="3">
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -1261,16 +1258,16 @@
         <v>3004</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D7" s="3">
         <v>15</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -1281,16 +1278,16 @@
         <v>3005</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D8" s="3">
         <v>15</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -1301,16 +1298,16 @@
         <v>3006</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D9" s="3">
         <v>15</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F9">
         <v>10</v>
@@ -1321,16 +1318,16 @@
         <v>3007</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D10" s="3">
         <v>15</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -1341,16 +1338,16 @@
         <v>3008</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D11" s="3">
         <v>15</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F11">
         <v>10</v>

</xml_diff>

<commit_message>
feat : Sound폴더 + 씬연결
</commit_message>
<xml_diff>
--- a/RawData/excel_files/DataTable.xlsx
+++ b/RawData/excel_files/DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Portfolio\Oilnam\RawData\excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grays\Desktop\Project\Unity\OIlNamProject\RawData\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46121667-A6DC-4D0B-AD8C-3F76981C9069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257CB841-604B-4B7A-A69D-B999AF33ED03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="880" windowWidth="19200" windowHeight="11170" activeTab="3" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter" sheetId="4" r:id="rId1"/>
@@ -988,15 +988,14 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="5" max="5" width="11.58203125" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.9140625" customWidth="1"/>
+    <col min="5" max="6" width="11.625" customWidth="1"/>
+    <col min="8" max="8" width="14.875" customWidth="1"/>
     <col min="9" max="9" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="13.5" customWidth="1"/>
     <col min="11" max="11" width="18.75" customWidth="1"/>
-    <col min="12" max="12" width="10.9140625" customWidth="1"/>
+    <col min="12" max="12" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1081,7 +1080,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17" customHeight="1">
+    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>37</v>
       </c>
@@ -3186,10 +3185,10 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="104.83203125" customWidth="1"/>
-    <col min="3" max="3" width="7.08203125" customWidth="1"/>
+    <col min="2" max="2" width="104.875" customWidth="1"/>
+    <col min="3" max="3" width="7.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3383,12 +3382,12 @@
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="8.58203125" customWidth="1"/>
-    <col min="3" max="3" width="22.58203125" customWidth="1"/>
-    <col min="4" max="4" width="14.4140625" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="8.625" customWidth="1"/>
+    <col min="3" max="3" width="22.625" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
+    <col min="5" max="5" width="20.125" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3432,7 +3431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.5" thickBot="1">
+    <row r="3" spans="1:6" ht="17.25" thickBot="1">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -3452,7 +3451,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.5" thickBot="1">
+    <row r="4" spans="1:6" ht="17.25" thickBot="1">
       <c r="A4" s="14">
         <v>401</v>
       </c>
@@ -3472,7 +3471,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.5" thickBot="1">
+    <row r="5" spans="1:6" ht="17.25" thickBot="1">
       <c r="A5" s="16">
         <v>402</v>
       </c>
@@ -3492,7 +3491,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.5" thickBot="1">
+    <row r="6" spans="1:6" ht="17.25" thickBot="1">
       <c r="A6" s="16">
         <v>403</v>
       </c>
@@ -3512,7 +3511,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.5" thickBot="1">
+    <row r="7" spans="1:6" ht="17.25" thickBot="1">
       <c r="A7" s="16">
         <v>404</v>
       </c>
@@ -3532,7 +3531,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.5" thickBot="1">
+    <row r="8" spans="1:6" ht="17.25" thickBot="1">
       <c r="A8" s="16">
         <v>405</v>
       </c>
@@ -3552,7 +3551,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.5" thickBot="1">
+    <row r="9" spans="1:6" ht="17.25" thickBot="1">
       <c r="A9" s="16">
         <v>406</v>
       </c>
@@ -3572,7 +3571,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.5" thickBot="1">
+    <row r="10" spans="1:6" ht="17.25" thickBot="1">
       <c r="A10" s="16">
         <v>407</v>
       </c>
@@ -3592,7 +3591,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17.5" thickBot="1">
+    <row r="11" spans="1:6" ht="17.25" thickBot="1">
       <c r="A11" s="16">
         <v>408</v>
       </c>
@@ -3612,7 +3611,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17.5" thickBot="1">
+    <row r="12" spans="1:6" ht="17.25" thickBot="1">
       <c r="A12" s="16">
         <v>409</v>
       </c>
@@ -3632,7 +3631,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.5" thickBot="1">
+    <row r="13" spans="1:6" ht="17.25" thickBot="1">
       <c r="A13" s="16">
         <v>410</v>
       </c>
@@ -3663,16 +3662,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B13BC7-908D-4893-B4AD-1079229E5F6F}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.58203125" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
+    <col min="5" max="5" width="20.625" customWidth="1"/>
+    <col min="6" max="6" width="13.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3715,7 +3714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.5" thickBot="1">
+    <row r="3" spans="1:6" ht="17.25" thickBot="1">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -3735,7 +3734,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.5" thickBot="1">
+    <row r="4" spans="1:6" ht="17.25" thickBot="1">
       <c r="A4" s="14">
         <v>501</v>
       </c>
@@ -3755,7 +3754,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.5" thickBot="1">
+    <row r="5" spans="1:6" ht="17.25" thickBot="1">
       <c r="A5" s="16">
         <v>502</v>
       </c>
@@ -3775,7 +3774,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.5" thickBot="1">
+    <row r="6" spans="1:6" ht="17.25" thickBot="1">
       <c r="A6" s="16">
         <v>503</v>
       </c>
@@ -3795,7 +3794,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.5" thickBot="1">
+    <row r="7" spans="1:6" ht="17.25" thickBot="1">
       <c r="A7" s="16">
         <v>504</v>
       </c>
@@ -3815,7 +3814,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.5" thickBot="1">
+    <row r="8" spans="1:6" ht="17.25" thickBot="1">
       <c r="A8" s="16">
         <v>505</v>
       </c>
@@ -3845,19 +3844,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40025AE-C7D8-4357-9319-EFD6B75D65B3}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="8.58203125" customWidth="1"/>
+    <col min="1" max="1" width="8.625" customWidth="1"/>
     <col min="2" max="2" width="42.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.58203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
fix : 스토리 database
(스토리 날라갔었네..)
</commit_message>
<xml_diff>
--- a/RawData/excel_files/DataTable.xlsx
+++ b/RawData/excel_files/DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grays\Desktop\Project\Unity\OIlNamProject\RawData\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5264E174-AF7A-4791-B899-F406C183A5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0E358A-15AF-442B-9292-3181E1B8214C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter" sheetId="4" r:id="rId1"/>
@@ -81,21 +81,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>큰 계약금을 제시하여 계약금에 홀린 헌터들을 협회에 묶어놓은 다음, 거액의 빚을 지게 하는 계약.</t>
-  </si>
-  <si>
-    <t>그래서 나는 그 빚을 갚기 위해 매일매일을 싸움터에서 뛰어다녀야 한다…</t>
-  </si>
-  <si>
-    <t>나에게는 아내를 똑 닮은 딸이 하나 있는데 매일 일하느라 엄마의 빈자리를 채워주지 못해서 미안하다…</t>
-  </si>
-  <si>
-    <t>하지만 빚을 갚기 위해서라도 계속 일을 해야 한다.</t>
-  </si>
-  <si>
-    <t>하…귀찮네…</t>
-  </si>
-  <si>
     <t>key</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -219,34 +204,6 @@
   </si>
   <si>
     <t>내딸이니까</t>
-  </si>
-  <si>
-    <t>&amp;&amp;전 세계에 균열이 발생했다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>차원 간의 균열이 열리며&amp;튀어나온 온갖 마물들은&amp;그야말로 자연재해였다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>하지만,&amp;인류는 멸망하지 않았다.&amp;&amp;균열에서 새어 나오는 마나를 받아들여 특별한 힘을 지니게 된 사람들 덕분이었다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내가 바로 그 힘을 가진&amp;'헌터'다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>나는 협회에 소속된 헌터다.&amp;그것도....&amp;헌터에 관련된 계약에 허점이 많은 시절에 계약하여 노예와 다름 없는 계약...</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(사이렌 소리)하… 또 균열이 발생했다.&amp;뭔 놈의 마물이 이렇게 하루가 멀다 하고 매일 나오는지 지겹다 지겨워…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(전화벨소리)왜?&amp;(중얼거리며) 아니...학교에서 필요한 준비물이 있는데..&amp;귀찮게 연락하지 말고, 카드로 사&amp;(뚝 끊음)&amp;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Energy1</t>
@@ -536,6 +493,87 @@
     <t>쓰읍... 아닐걸?
 다시 한 번
 잘 생각해봐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+전 세계에 균열이 발생했다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내가 바로
+그 힘을 가진
+'헌터'다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나는 협회에 소속된 헌터다.
+그것도....
+헌터에 관련된 계약에
+허점이 많은 시절에 계약하여
+노예와 다름 없는 계약…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>큰 계약금을 제시하여
+계약금에 홀린 헌터들을
+협회에 묶어놓은 다음,
+거액의 빚을 지게 하는 계약.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나는 그 빚을 갚기 위해
+매일매일을 싸움터에서
+뛰어다녀야 한다…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나에게는
+아내를 똑 닮은 딸이 하나 있는데
+매일 일하느라 엄마의 빈자리를
+채워주지 못해서 미안하다…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하지만 빚을 갚기 위해서
+계속 일은 해야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(사이렌 소리)
+하…
+또 균열이 발생했다.
+뭔 놈의 마물이
+이렇게 하루가 멀다 하고
+매일 나오는지…
+지겹다 지겨워…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(전화벨소리)왜?
+(중얼거리며) 아빠...학교에서 필요한 준비물이 있는데..
+귀찮게 연락하지 말고,
+카드로 사
+(뚝 끊음)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하… 다 귀찮네…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>차원 간의 균열이 열리며
+튀어나온 온갖 마물들은
+그야말로
+자연재해
+그 자체였다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하지만,
+인류는 멸망하지 않았다.
+균열에서 새어 나오는 마나를 받아들여
+특별한 힘을 지니게 된 사람들 덕분이었다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -702,7 +740,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -762,6 +800,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1095,125 +1136,125 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="H1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="I1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="J1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="K1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="L1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="M1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="I3" s="5" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -3276,8 +3317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8FABB6-B12D-4D0B-ADBA-E809D3A5F66E}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3288,7 +3329,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -3299,13 +3340,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3330,122 +3371,122 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" ht="49.5">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
-        <v>55</v>
+      <c r="B5" s="20" t="s">
+        <v>125</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" ht="82.5">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>56</v>
+      <c r="B6" s="20" t="s">
+        <v>135</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" ht="82.5">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>57</v>
+      <c r="B7" s="20" t="s">
+        <v>136</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" ht="49.5">
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
-        <v>58</v>
+      <c r="B8" s="20" t="s">
+        <v>126</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" ht="82.5">
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
-        <v>59</v>
+      <c r="B9" s="20" t="s">
+        <v>127</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" ht="66">
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
-        <v>15</v>
+      <c r="B10" s="20" t="s">
+        <v>128</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" ht="49.5">
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
-        <v>16</v>
+      <c r="B11" s="20" t="s">
+        <v>129</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" ht="66">
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" t="s">
-        <v>17</v>
+      <c r="B12" s="20" t="s">
+        <v>130</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" ht="33">
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
-        <v>18</v>
+      <c r="B13" s="20" t="s">
+        <v>131</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" ht="115.5">
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14" t="s">
-        <v>60</v>
+      <c r="B14" s="20" t="s">
+        <v>132</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" ht="82.5">
       <c r="A15">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
-        <v>61</v>
+      <c r="B15" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>14</v>
@@ -3456,7 +3497,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>134</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -3488,22 +3529,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3528,22 +3569,22 @@
     </row>
     <row r="3" spans="1:6" ht="17.25" thickBot="1">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17.25" thickBot="1">
@@ -3563,7 +3604,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.25" thickBot="1">
@@ -3583,7 +3624,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17.25" thickBot="1">
@@ -3603,7 +3644,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17.25" thickBot="1">
@@ -3623,7 +3664,7 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17.25" thickBot="1">
@@ -3643,7 +3684,7 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17.25" thickBot="1">
@@ -3651,7 +3692,7 @@
         <v>406</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C9" s="17">
         <v>1</v>
@@ -3663,7 +3704,7 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17.25" thickBot="1">
@@ -3671,7 +3712,7 @@
         <v>407</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C10" s="17">
         <v>1</v>
@@ -3683,7 +3724,7 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17.25" thickBot="1">
@@ -3691,7 +3732,7 @@
         <v>408</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C11" s="17">
         <v>1</v>
@@ -3703,7 +3744,7 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17.25" thickBot="1">
@@ -3711,7 +3752,7 @@
         <v>409</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C12" s="17">
         <v>1</v>
@@ -3723,7 +3764,7 @@
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25" thickBot="1">
@@ -3731,7 +3772,7 @@
         <v>410</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C13" s="17">
         <v>1</v>
@@ -3743,7 +3784,7 @@
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3771,22 +3812,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3811,22 +3852,22 @@
     </row>
     <row r="3" spans="1:6" ht="17.25" thickBot="1">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17.25" thickBot="1">
@@ -3834,7 +3875,7 @@
         <v>501</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C4" s="15">
         <v>1</v>
@@ -3846,7 +3887,7 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.25" thickBot="1">
@@ -3854,7 +3895,7 @@
         <v>502</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C5" s="17">
         <v>1</v>
@@ -3866,7 +3907,7 @@
         <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17.25" thickBot="1">
@@ -3874,7 +3915,7 @@
         <v>503</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C6" s="17">
         <v>1</v>
@@ -3886,7 +3927,7 @@
         <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17.25" thickBot="1">
@@ -3894,7 +3935,7 @@
         <v>504</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C7" s="17">
         <v>1</v>
@@ -3906,7 +3947,7 @@
         <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17.25" thickBot="1">
@@ -3914,7 +3955,7 @@
         <v>505</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C8" s="17">
         <v>1</v>
@@ -3926,7 +3967,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -3939,7 +3980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40025AE-C7D8-4357-9319-EFD6B75D65B3}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -3964,58 +4005,58 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="N1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -4023,108 +4064,108 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="K2" t="s">
         <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="N2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="O2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="P2" t="s">
         <v>2</v>
       </c>
       <c r="Q2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="R2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>10</v>
@@ -4135,16 +4176,16 @@
         <v>3001</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F4" s="3">
         <v>20</v>
@@ -4153,13 +4194,13 @@
         <v>-15</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="K4">
         <v>-10</v>
@@ -4168,13 +4209,13 @@
         <v>20</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="P4">
         <v>30</v>
@@ -4183,7 +4224,7 @@
         <v>-15</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="49.5">
@@ -4191,16 +4232,16 @@
         <v>3002</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F5" s="3">
         <v>20</v>
@@ -4209,13 +4250,13 @@
         <v>-15</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="K5">
         <v>-10</v>
@@ -4224,13 +4265,13 @@
         <v>20</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="O5" s="19" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="P5">
         <v>30</v>
@@ -4239,7 +4280,7 @@
         <v>-15</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="66">
@@ -4247,16 +4288,16 @@
         <v>3003</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F6" s="3">
         <v>20</v>
@@ -4265,13 +4306,13 @@
         <v>-15</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="K6">
         <v>-10</v>
@@ -4280,13 +4321,13 @@
         <v>20</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="O6" s="19" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="P6">
         <v>30</v>
@@ -4295,7 +4336,7 @@
         <v>-15</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="49.5">
@@ -4303,16 +4344,16 @@
         <v>3004</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F7" s="3">
         <v>20</v>
@@ -4321,13 +4362,13 @@
         <v>-15</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="K7">
         <v>-10</v>
@@ -4336,13 +4377,13 @@
         <v>20</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="O7" s="19" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="P7">
         <v>30</v>
@@ -4351,7 +4392,7 @@
         <v>-15</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="49.5">
@@ -4359,16 +4400,16 @@
         <v>3005</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="F8" s="3">
         <v>20</v>
@@ -4377,13 +4418,13 @@
         <v>-15</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="K8">
         <v>-10</v>
@@ -4392,13 +4433,13 @@
         <v>20</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="O8" s="19" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="P8">
         <v>30</v>
@@ -4407,7 +4448,7 @@
         <v>-15</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="49.5">
@@ -4415,16 +4456,16 @@
         <v>3006</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F9" s="3">
         <v>20</v>
@@ -4433,13 +4474,13 @@
         <v>-15</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="K9">
         <v>-10</v>
@@ -4448,13 +4489,13 @@
         <v>20</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="O9" s="19" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="P9">
         <v>30</v>
@@ -4463,7 +4504,7 @@
         <v>-15</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="49.5">
@@ -4471,16 +4512,16 @@
         <v>3007</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F10" s="3">
         <v>20</v>
@@ -4489,13 +4530,13 @@
         <v>-15</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="K10">
         <v>-10</v>
@@ -4504,13 +4545,13 @@
         <v>20</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="P10">
         <v>30</v>
@@ -4519,7 +4560,7 @@
         <v>-15</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="49.5">
@@ -4527,16 +4568,16 @@
         <v>3008</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F11" s="3">
         <v>20</v>
@@ -4545,13 +4586,13 @@
         <v>-15</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="K11">
         <v>-10</v>
@@ -4560,13 +4601,13 @@
         <v>20</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="O11" s="19" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="P11">
         <v>30</v>
@@ -4575,7 +4616,7 @@
         <v>-15</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "feat : UnitManager"
This reverts commit 9ac008a0a8198c4fbec7f5ecdada95b06fdde369.
</commit_message>
<xml_diff>
--- a/RawData/excel_files/DataTable.xlsx
+++ b/RawData/excel_files/DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grays\Desktop\Project\Unity\OIlNamProject\RawData\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C03177-41D9-4235-9C40-295C73EFD9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36379A7-9C58-4FE4-8CA0-65CA0BA0BF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34515" yWindow="1785" windowWidth="20010" windowHeight="11385" activeTab="6" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter" sheetId="4" r:id="rId1"/>
@@ -18,8 +18,6 @@
     <sheet name="Enemy" sheetId="1" r:id="rId3"/>
     <sheet name="Boss" sheetId="5" r:id="rId4"/>
     <sheet name="Message" sheetId="3" r:id="rId5"/>
-    <sheet name="Unit" sheetId="6" r:id="rId6"/>
-    <sheet name="Upgrade" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="132">
   <si>
     <t>Name</t>
   </si>
@@ -556,254 +554,6 @@
 인류는 멸망하지 않았다.
 균열에서 새어 나오는 마나를 받아들여
 특별한 힘을 지니게 된 사람들 덕분이었다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unit_Tier</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>ATK</t>
-  </si>
-  <si>
-    <t>Attack_Speed</t>
-  </si>
-  <si>
-    <t>Attack_Range</t>
-  </si>
-  <si>
-    <t>Unit_Modeling</t>
-  </si>
-  <si>
-    <t>가브리엘</t>
-  </si>
-  <si>
-    <t>세계를 구한 7대 영웅 중 1명입니다.</t>
-  </si>
-  <si>
-    <t>SS1_gif</t>
-  </si>
-  <si>
-    <t>잉그리드</t>
-  </si>
-  <si>
-    <t>SS2_gif</t>
-  </si>
-  <si>
-    <t>제이드</t>
-  </si>
-  <si>
-    <t>실력이 뛰어난 검사입니다.</t>
-  </si>
-  <si>
-    <t>SA3_gif</t>
-  </si>
-  <si>
-    <t>리</t>
-  </si>
-  <si>
-    <t>SA4_gif</t>
-  </si>
-  <si>
-    <t>잭슨</t>
-  </si>
-  <si>
-    <t>견습 검사입니다.</t>
-  </si>
-  <si>
-    <t>SB5_gif</t>
-  </si>
-  <si>
-    <t>잭</t>
-  </si>
-  <si>
-    <t>SB6_gif</t>
-  </si>
-  <si>
-    <t>칼리</t>
-  </si>
-  <si>
-    <t>AS1_gif</t>
-  </si>
-  <si>
-    <t>엘린</t>
-  </si>
-  <si>
-    <t>AS2_gif</t>
-  </si>
-  <si>
-    <t>체이스</t>
-  </si>
-  <si>
-    <t>실력이 뛰어난 궁수입니다.</t>
-  </si>
-  <si>
-    <t>AA3_gif</t>
-  </si>
-  <si>
-    <t>파벨</t>
-  </si>
-  <si>
-    <t>AA4_gif</t>
-  </si>
-  <si>
-    <t>매기</t>
-  </si>
-  <si>
-    <t>견습 궁수입니다.</t>
-  </si>
-  <si>
-    <t>AB5_gif</t>
-  </si>
-  <si>
-    <t>마돈나</t>
-  </si>
-  <si>
-    <t>AB6_gif</t>
-  </si>
-  <si>
-    <t>에반</t>
-  </si>
-  <si>
-    <t>WS1_gif</t>
-  </si>
-  <si>
-    <t>밤비</t>
-  </si>
-  <si>
-    <t>WS2_gif</t>
-  </si>
-  <si>
-    <t>오로라</t>
-  </si>
-  <si>
-    <t>WS3_gif</t>
-  </si>
-  <si>
-    <t>데이브</t>
-  </si>
-  <si>
-    <t>실력이 뛰어난 마법사입니다.</t>
-  </si>
-  <si>
-    <t>WA4_gif</t>
-  </si>
-  <si>
-    <t>데이지</t>
-  </si>
-  <si>
-    <t>WA5_gif</t>
-  </si>
-  <si>
-    <t>콜린</t>
-  </si>
-  <si>
-    <t>WA6_gif</t>
-  </si>
-  <si>
-    <t>아만다</t>
-  </si>
-  <si>
-    <t>견습 마법사입니다.</t>
-  </si>
-  <si>
-    <t>WB7_gif</t>
-  </si>
-  <si>
-    <t>오스카</t>
-  </si>
-  <si>
-    <t>WB8_gif</t>
-  </si>
-  <si>
-    <t>헤스티아</t>
-  </si>
-  <si>
-    <t>WB9_gif</t>
-  </si>
-  <si>
-    <t>Open</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>false</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>rue</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>UnitID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unit ID</t>
-  </si>
-  <si>
-    <t>Tier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ATK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12,23,34,45,56,67,78</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12,23,34,45,56,67,79</t>
-  </si>
-  <si>
-    <t>12,23,34,45,56,67,80</t>
-  </si>
-  <si>
-    <t>List&lt;int&gt;</t>
-  </si>
-  <si>
-    <t>List&lt;int&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Drop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NeedPiece</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1,2,3,4,5,6,7</t>
-  </si>
-  <si>
-    <t>1,2,3,4,5,6,7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -970,7 +720,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1033,9 +783,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3550,7 +3297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8FABB6-B12D-4D0B-ADBA-E809D3A5F66E}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -3748,7 +3495,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4213,7 +3960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40025AE-C7D8-4357-9319-EFD6B75D65B3}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
@@ -4756,1298 +4503,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3B3B7E-BA51-4E15-824F-73A2BFC53D10}">
-  <dimension ref="A1:I24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <cols>
-    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H1" t="s">
-        <v>187</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F3" t="s">
-        <v>135</v>
-      </c>
-      <c r="G3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="I3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4">
-        <v>201</v>
-      </c>
-      <c r="B4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E4">
-        <v>43</v>
-      </c>
-      <c r="F4">
-        <v>9500</v>
-      </c>
-      <c r="G4">
-        <v>280</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="I4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5">
-        <v>202</v>
-      </c>
-      <c r="B5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5">
-        <v>37</v>
-      </c>
-      <c r="F5">
-        <v>8700</v>
-      </c>
-      <c r="G5">
-        <v>280</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="I5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6">
-        <v>203</v>
-      </c>
-      <c r="B6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6">
-        <v>32</v>
-      </c>
-      <c r="F6">
-        <v>10600</v>
-      </c>
-      <c r="G6">
-        <v>260</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="I6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7">
-        <v>204</v>
-      </c>
-      <c r="B7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E7">
-        <v>26</v>
-      </c>
-      <c r="F7">
-        <v>9800</v>
-      </c>
-      <c r="G7">
-        <v>260</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8">
-        <v>205</v>
-      </c>
-      <c r="B8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>149</v>
-      </c>
-      <c r="E8">
-        <v>20</v>
-      </c>
-      <c r="F8">
-        <v>13000</v>
-      </c>
-      <c r="G8">
-        <v>240</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9">
-        <v>206</v>
-      </c>
-      <c r="B9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E9">
-        <v>14</v>
-      </c>
-      <c r="F9">
-        <v>12000</v>
-      </c>
-      <c r="G9">
-        <v>240</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10">
-        <v>207</v>
-      </c>
-      <c r="B10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>139</v>
-      </c>
-      <c r="E10">
-        <v>22</v>
-      </c>
-      <c r="F10">
-        <v>5200</v>
-      </c>
-      <c r="G10">
-        <v>350</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11">
-        <v>208</v>
-      </c>
-      <c r="B11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>139</v>
-      </c>
-      <c r="E11">
-        <v>18</v>
-      </c>
-      <c r="F11">
-        <v>4300</v>
-      </c>
-      <c r="G11">
-        <v>350</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12">
-        <v>209</v>
-      </c>
-      <c r="B12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>158</v>
-      </c>
-      <c r="E12">
-        <v>18</v>
-      </c>
-      <c r="F12">
-        <v>6300</v>
-      </c>
-      <c r="G12">
-        <v>320</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13">
-        <v>210</v>
-      </c>
-      <c r="B13" t="s">
-        <v>160</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>158</v>
-      </c>
-      <c r="E13">
-        <v>15</v>
-      </c>
-      <c r="F13">
-        <v>5600</v>
-      </c>
-      <c r="G13">
-        <v>320</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14">
-        <v>211</v>
-      </c>
-      <c r="B14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>163</v>
-      </c>
-      <c r="E14">
-        <v>17</v>
-      </c>
-      <c r="F14">
-        <v>7200</v>
-      </c>
-      <c r="G14">
-        <v>300</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I14" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15">
-        <v>212</v>
-      </c>
-      <c r="B15" t="s">
-        <v>165</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15" t="s">
-        <v>163</v>
-      </c>
-      <c r="E15">
-        <v>14</v>
-      </c>
-      <c r="F15">
-        <v>7800</v>
-      </c>
-      <c r="G15">
-        <v>300</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16">
-        <v>213</v>
-      </c>
-      <c r="B16" t="s">
-        <v>167</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>139</v>
-      </c>
-      <c r="E16">
-        <v>45</v>
-      </c>
-      <c r="F16">
-        <v>10300</v>
-      </c>
-      <c r="G16">
-        <v>410</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I16" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17">
-        <v>214</v>
-      </c>
-      <c r="B17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>139</v>
-      </c>
-      <c r="E17">
-        <v>40</v>
-      </c>
-      <c r="F17">
-        <v>9900</v>
-      </c>
-      <c r="G17">
-        <v>400</v>
-      </c>
-      <c r="H17" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I17" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18">
-        <v>215</v>
-      </c>
-      <c r="B18" t="s">
-        <v>171</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>139</v>
-      </c>
-      <c r="E18">
-        <v>48</v>
-      </c>
-      <c r="F18">
-        <v>12400</v>
-      </c>
-      <c r="G18">
-        <v>430</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19">
-        <v>216</v>
-      </c>
-      <c r="B19" t="s">
-        <v>173</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>174</v>
-      </c>
-      <c r="E19">
-        <v>33</v>
-      </c>
-      <c r="F19">
-        <v>11200</v>
-      </c>
-      <c r="G19">
-        <v>370</v>
-      </c>
-      <c r="H19" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I19" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20">
-        <v>217</v>
-      </c>
-      <c r="B20" t="s">
-        <v>176</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>174</v>
-      </c>
-      <c r="E20">
-        <v>28</v>
-      </c>
-      <c r="F20">
-        <v>10800</v>
-      </c>
-      <c r="G20">
-        <v>360</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I20" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21">
-        <v>218</v>
-      </c>
-      <c r="B21" t="s">
-        <v>178</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>174</v>
-      </c>
-      <c r="E21">
-        <v>36</v>
-      </c>
-      <c r="F21">
-        <v>12300</v>
-      </c>
-      <c r="G21">
-        <v>390</v>
-      </c>
-      <c r="H21" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I21" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22">
-        <v>219</v>
-      </c>
-      <c r="B22" t="s">
-        <v>180</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22" t="s">
-        <v>181</v>
-      </c>
-      <c r="E22">
-        <v>27</v>
-      </c>
-      <c r="F22">
-        <v>12600</v>
-      </c>
-      <c r="G22">
-        <v>360</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I22" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23">
-        <v>220</v>
-      </c>
-      <c r="B23" t="s">
-        <v>183</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23" t="s">
-        <v>181</v>
-      </c>
-      <c r="E23">
-        <v>22</v>
-      </c>
-      <c r="F23">
-        <v>13600</v>
-      </c>
-      <c r="G23">
-        <v>350</v>
-      </c>
-      <c r="H23" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I23" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24">
-        <v>221</v>
-      </c>
-      <c r="B24" t="s">
-        <v>185</v>
-      </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-      <c r="D24" t="s">
-        <v>181</v>
-      </c>
-      <c r="E24">
-        <v>30</v>
-      </c>
-      <c r="F24">
-        <v>14600</v>
-      </c>
-      <c r="G24">
-        <v>380</v>
-      </c>
-      <c r="H24" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I24" t="s">
-        <v>186</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246DAC17-E872-4574-BD3D-D5CF034B9B32}">
-  <dimension ref="A1:G24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <cols>
-    <col min="3" max="5" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>195</v>
-      </c>
-      <c r="F1" t="s">
-        <v>201</v>
-      </c>
-      <c r="G1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E2" t="s">
-        <v>200</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>202</v>
-      </c>
-      <c r="G3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
-        <v>801</v>
-      </c>
-      <c r="B4">
-        <v>201</v>
-      </c>
-      <c r="C4" t="s">
-        <v>196</v>
-      </c>
-      <c r="D4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E4" t="s">
-        <v>198</v>
-      </c>
-      <c r="F4">
-        <v>140</v>
-      </c>
-      <c r="G4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>802</v>
-      </c>
-      <c r="B5">
-        <v>202</v>
-      </c>
-      <c r="C5" t="s">
-        <v>196</v>
-      </c>
-      <c r="D5" t="s">
-        <v>197</v>
-      </c>
-      <c r="E5" t="s">
-        <v>198</v>
-      </c>
-      <c r="F5">
-        <v>140</v>
-      </c>
-      <c r="G5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>803</v>
-      </c>
-      <c r="B6">
-        <v>203</v>
-      </c>
-      <c r="C6" t="s">
-        <v>196</v>
-      </c>
-      <c r="D6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F6">
-        <v>355</v>
-      </c>
-      <c r="G6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>804</v>
-      </c>
-      <c r="B7">
-        <v>204</v>
-      </c>
-      <c r="C7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D7" t="s">
-        <v>197</v>
-      </c>
-      <c r="E7" t="s">
-        <v>198</v>
-      </c>
-      <c r="F7">
-        <v>355</v>
-      </c>
-      <c r="G7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
-        <v>805</v>
-      </c>
-      <c r="B8">
-        <v>205</v>
-      </c>
-      <c r="C8" t="s">
-        <v>196</v>
-      </c>
-      <c r="D8" t="s">
-        <v>197</v>
-      </c>
-      <c r="E8" t="s">
-        <v>198</v>
-      </c>
-      <c r="F8">
-        <v>933</v>
-      </c>
-      <c r="G8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>806</v>
-      </c>
-      <c r="B9">
-        <v>206</v>
-      </c>
-      <c r="C9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" t="s">
-        <v>197</v>
-      </c>
-      <c r="E9" t="s">
-        <v>198</v>
-      </c>
-      <c r="F9">
-        <v>933</v>
-      </c>
-      <c r="G9" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <v>807</v>
-      </c>
-      <c r="B10">
-        <v>207</v>
-      </c>
-      <c r="C10" t="s">
-        <v>196</v>
-      </c>
-      <c r="D10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E10" t="s">
-        <v>198</v>
-      </c>
-      <c r="F10">
-        <v>140</v>
-      </c>
-      <c r="G10" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
-        <v>808</v>
-      </c>
-      <c r="B11">
-        <v>208</v>
-      </c>
-      <c r="C11" t="s">
-        <v>196</v>
-      </c>
-      <c r="D11" t="s">
-        <v>197</v>
-      </c>
-      <c r="E11" t="s">
-        <v>198</v>
-      </c>
-      <c r="F11">
-        <v>140</v>
-      </c>
-      <c r="G11" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
-        <v>809</v>
-      </c>
-      <c r="B12">
-        <v>209</v>
-      </c>
-      <c r="C12" t="s">
-        <v>196</v>
-      </c>
-      <c r="D12" t="s">
-        <v>197</v>
-      </c>
-      <c r="E12" t="s">
-        <v>198</v>
-      </c>
-      <c r="F12">
-        <v>355</v>
-      </c>
-      <c r="G12" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
-        <v>810</v>
-      </c>
-      <c r="B13">
-        <v>210</v>
-      </c>
-      <c r="C13" t="s">
-        <v>196</v>
-      </c>
-      <c r="D13" t="s">
-        <v>197</v>
-      </c>
-      <c r="E13" t="s">
-        <v>198</v>
-      </c>
-      <c r="F13">
-        <v>355</v>
-      </c>
-      <c r="G13" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
-        <v>811</v>
-      </c>
-      <c r="B14">
-        <v>211</v>
-      </c>
-      <c r="C14" t="s">
-        <v>196</v>
-      </c>
-      <c r="D14" t="s">
-        <v>197</v>
-      </c>
-      <c r="E14" t="s">
-        <v>198</v>
-      </c>
-      <c r="F14">
-        <v>933</v>
-      </c>
-      <c r="G14" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15">
-        <v>812</v>
-      </c>
-      <c r="B15">
-        <v>212</v>
-      </c>
-      <c r="C15" t="s">
-        <v>196</v>
-      </c>
-      <c r="D15" t="s">
-        <v>197</v>
-      </c>
-      <c r="E15" t="s">
-        <v>198</v>
-      </c>
-      <c r="F15">
-        <v>933</v>
-      </c>
-      <c r="G15" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16">
-        <v>813</v>
-      </c>
-      <c r="B16">
-        <v>213</v>
-      </c>
-      <c r="C16" t="s">
-        <v>196</v>
-      </c>
-      <c r="D16" t="s">
-        <v>197</v>
-      </c>
-      <c r="E16" t="s">
-        <v>198</v>
-      </c>
-      <c r="F16">
-        <v>140</v>
-      </c>
-      <c r="G16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17">
-        <v>814</v>
-      </c>
-      <c r="B17">
-        <v>214</v>
-      </c>
-      <c r="C17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D17" t="s">
-        <v>197</v>
-      </c>
-      <c r="E17" t="s">
-        <v>198</v>
-      </c>
-      <c r="F17">
-        <v>140</v>
-      </c>
-      <c r="G17" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18">
-        <v>815</v>
-      </c>
-      <c r="B18">
-        <v>215</v>
-      </c>
-      <c r="C18" t="s">
-        <v>196</v>
-      </c>
-      <c r="D18" t="s">
-        <v>197</v>
-      </c>
-      <c r="E18" t="s">
-        <v>198</v>
-      </c>
-      <c r="F18">
-        <v>140</v>
-      </c>
-      <c r="G18" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19">
-        <v>816</v>
-      </c>
-      <c r="B19">
-        <v>216</v>
-      </c>
-      <c r="C19" t="s">
-        <v>196</v>
-      </c>
-      <c r="D19" t="s">
-        <v>197</v>
-      </c>
-      <c r="E19" t="s">
-        <v>198</v>
-      </c>
-      <c r="F19">
-        <v>355</v>
-      </c>
-      <c r="G19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20">
-        <v>817</v>
-      </c>
-      <c r="B20">
-        <v>217</v>
-      </c>
-      <c r="C20" t="s">
-        <v>196</v>
-      </c>
-      <c r="D20" t="s">
-        <v>197</v>
-      </c>
-      <c r="E20" t="s">
-        <v>198</v>
-      </c>
-      <c r="F20">
-        <v>355</v>
-      </c>
-      <c r="G20" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21">
-        <v>818</v>
-      </c>
-      <c r="B21">
-        <v>218</v>
-      </c>
-      <c r="C21" t="s">
-        <v>196</v>
-      </c>
-      <c r="D21" t="s">
-        <v>197</v>
-      </c>
-      <c r="E21" t="s">
-        <v>198</v>
-      </c>
-      <c r="F21">
-        <v>355</v>
-      </c>
-      <c r="G21" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22">
-        <v>819</v>
-      </c>
-      <c r="B22">
-        <v>219</v>
-      </c>
-      <c r="C22" t="s">
-        <v>196</v>
-      </c>
-      <c r="D22" t="s">
-        <v>197</v>
-      </c>
-      <c r="E22" t="s">
-        <v>198</v>
-      </c>
-      <c r="F22">
-        <v>933</v>
-      </c>
-      <c r="G22" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23">
-        <v>820</v>
-      </c>
-      <c r="B23">
-        <v>220</v>
-      </c>
-      <c r="C23" t="s">
-        <v>196</v>
-      </c>
-      <c r="D23" t="s">
-        <v>197</v>
-      </c>
-      <c r="E23" t="s">
-        <v>198</v>
-      </c>
-      <c r="F23">
-        <v>933</v>
-      </c>
-      <c r="G23" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24">
-        <v>821</v>
-      </c>
-      <c r="B24">
-        <v>221</v>
-      </c>
-      <c r="C24" t="s">
-        <v>196</v>
-      </c>
-      <c r="D24" t="s">
-        <v>197</v>
-      </c>
-      <c r="E24" t="s">
-        <v>198</v>
-      </c>
-      <c r="F24">
-        <v>933</v>
-      </c>
-      <c r="G24" t="s">
-        <v>204</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Reapply "feat : UnitManager"
This reverts commit 7261e2c7113e6b2efbd5a5122fae7dc147d0cf1f.
</commit_message>
<xml_diff>
--- a/RawData/excel_files/DataTable.xlsx
+++ b/RawData/excel_files/DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grays\Desktop\Project\Unity\OIlNamProject\RawData\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36379A7-9C58-4FE4-8CA0-65CA0BA0BF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C03177-41D9-4235-9C40-295C73EFD9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
+    <workbookView xWindow="34515" yWindow="1785" windowWidth="20010" windowHeight="11385" activeTab="6" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Enemy" sheetId="1" r:id="rId3"/>
     <sheet name="Boss" sheetId="5" r:id="rId4"/>
     <sheet name="Message" sheetId="3" r:id="rId5"/>
+    <sheet name="Unit" sheetId="6" r:id="rId6"/>
+    <sheet name="Upgrade" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="206">
   <si>
     <t>Name</t>
   </si>
@@ -554,6 +556,254 @@
 인류는 멸망하지 않았다.
 균열에서 새어 나오는 마나를 받아들여
 특별한 힘을 지니게 된 사람들 덕분이었다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit_Tier</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ATK</t>
+  </si>
+  <si>
+    <t>Attack_Speed</t>
+  </si>
+  <si>
+    <t>Attack_Range</t>
+  </si>
+  <si>
+    <t>Unit_Modeling</t>
+  </si>
+  <si>
+    <t>가브리엘</t>
+  </si>
+  <si>
+    <t>세계를 구한 7대 영웅 중 1명입니다.</t>
+  </si>
+  <si>
+    <t>SS1_gif</t>
+  </si>
+  <si>
+    <t>잉그리드</t>
+  </si>
+  <si>
+    <t>SS2_gif</t>
+  </si>
+  <si>
+    <t>제이드</t>
+  </si>
+  <si>
+    <t>실력이 뛰어난 검사입니다.</t>
+  </si>
+  <si>
+    <t>SA3_gif</t>
+  </si>
+  <si>
+    <t>리</t>
+  </si>
+  <si>
+    <t>SA4_gif</t>
+  </si>
+  <si>
+    <t>잭슨</t>
+  </si>
+  <si>
+    <t>견습 검사입니다.</t>
+  </si>
+  <si>
+    <t>SB5_gif</t>
+  </si>
+  <si>
+    <t>잭</t>
+  </si>
+  <si>
+    <t>SB6_gif</t>
+  </si>
+  <si>
+    <t>칼리</t>
+  </si>
+  <si>
+    <t>AS1_gif</t>
+  </si>
+  <si>
+    <t>엘린</t>
+  </si>
+  <si>
+    <t>AS2_gif</t>
+  </si>
+  <si>
+    <t>체이스</t>
+  </si>
+  <si>
+    <t>실력이 뛰어난 궁수입니다.</t>
+  </si>
+  <si>
+    <t>AA3_gif</t>
+  </si>
+  <si>
+    <t>파벨</t>
+  </si>
+  <si>
+    <t>AA4_gif</t>
+  </si>
+  <si>
+    <t>매기</t>
+  </si>
+  <si>
+    <t>견습 궁수입니다.</t>
+  </si>
+  <si>
+    <t>AB5_gif</t>
+  </si>
+  <si>
+    <t>마돈나</t>
+  </si>
+  <si>
+    <t>AB6_gif</t>
+  </si>
+  <si>
+    <t>에반</t>
+  </si>
+  <si>
+    <t>WS1_gif</t>
+  </si>
+  <si>
+    <t>밤비</t>
+  </si>
+  <si>
+    <t>WS2_gif</t>
+  </si>
+  <si>
+    <t>오로라</t>
+  </si>
+  <si>
+    <t>WS3_gif</t>
+  </si>
+  <si>
+    <t>데이브</t>
+  </si>
+  <si>
+    <t>실력이 뛰어난 마법사입니다.</t>
+  </si>
+  <si>
+    <t>WA4_gif</t>
+  </si>
+  <si>
+    <t>데이지</t>
+  </si>
+  <si>
+    <t>WA5_gif</t>
+  </si>
+  <si>
+    <t>콜린</t>
+  </si>
+  <si>
+    <t>WA6_gif</t>
+  </si>
+  <si>
+    <t>아만다</t>
+  </si>
+  <si>
+    <t>견습 마법사입니다.</t>
+  </si>
+  <si>
+    <t>WB7_gif</t>
+  </si>
+  <si>
+    <t>오스카</t>
+  </si>
+  <si>
+    <t>WB8_gif</t>
+  </si>
+  <si>
+    <t>헤스티아</t>
+  </si>
+  <si>
+    <t>WB9_gif</t>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>rue</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UnitID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit ID</t>
+  </si>
+  <si>
+    <t>Tier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12,23,34,45,56,67,78</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12,23,34,45,56,67,79</t>
+  </si>
+  <si>
+    <t>12,23,34,45,56,67,80</t>
+  </si>
+  <si>
+    <t>List&lt;int&gt;</t>
+  </si>
+  <si>
+    <t>List&lt;int&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Drop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeedPiece</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -720,7 +970,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -783,6 +1033,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3297,7 +3550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8FABB6-B12D-4D0B-ADBA-E809D3A5F66E}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -3495,7 +3748,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3960,7 +4213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40025AE-C7D8-4357-9319-EFD6B75D65B3}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
@@ -4503,4 +4756,1298 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3B3B7E-BA51-4E15-824F-73A2BFC53D10}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>201</v>
+      </c>
+      <c r="B4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4">
+        <v>43</v>
+      </c>
+      <c r="F4">
+        <v>9500</v>
+      </c>
+      <c r="G4">
+        <v>280</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="I4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>202</v>
+      </c>
+      <c r="B5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5">
+        <v>37</v>
+      </c>
+      <c r="F5">
+        <v>8700</v>
+      </c>
+      <c r="G5">
+        <v>280</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="I5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>203</v>
+      </c>
+      <c r="B6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6">
+        <v>32</v>
+      </c>
+      <c r="F6">
+        <v>10600</v>
+      </c>
+      <c r="G6">
+        <v>260</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="I6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>204</v>
+      </c>
+      <c r="B7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7">
+        <v>26</v>
+      </c>
+      <c r="F7">
+        <v>9800</v>
+      </c>
+      <c r="G7">
+        <v>260</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>205</v>
+      </c>
+      <c r="B8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>13000</v>
+      </c>
+      <c r="G8">
+        <v>240</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>206</v>
+      </c>
+      <c r="B9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>12000</v>
+      </c>
+      <c r="G9">
+        <v>240</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>207</v>
+      </c>
+      <c r="B10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10">
+        <v>22</v>
+      </c>
+      <c r="F10">
+        <v>5200</v>
+      </c>
+      <c r="G10">
+        <v>350</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>208</v>
+      </c>
+      <c r="B11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11">
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <v>4300</v>
+      </c>
+      <c r="G11">
+        <v>350</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>209</v>
+      </c>
+      <c r="B12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12">
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>6300</v>
+      </c>
+      <c r="G12">
+        <v>320</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>210</v>
+      </c>
+      <c r="B13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>5600</v>
+      </c>
+      <c r="G13">
+        <v>320</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>211</v>
+      </c>
+      <c r="B14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14">
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>7200</v>
+      </c>
+      <c r="G14">
+        <v>300</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>212</v>
+      </c>
+      <c r="B15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="F15">
+        <v>7800</v>
+      </c>
+      <c r="G15">
+        <v>300</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>213</v>
+      </c>
+      <c r="B16" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16">
+        <v>45</v>
+      </c>
+      <c r="F16">
+        <v>10300</v>
+      </c>
+      <c r="G16">
+        <v>410</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>214</v>
+      </c>
+      <c r="B17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E17">
+        <v>40</v>
+      </c>
+      <c r="F17">
+        <v>9900</v>
+      </c>
+      <c r="G17">
+        <v>400</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18">
+        <v>215</v>
+      </c>
+      <c r="B18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>139</v>
+      </c>
+      <c r="E18">
+        <v>48</v>
+      </c>
+      <c r="F18">
+        <v>12400</v>
+      </c>
+      <c r="G18">
+        <v>430</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19">
+        <v>216</v>
+      </c>
+      <c r="B19" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>174</v>
+      </c>
+      <c r="E19">
+        <v>33</v>
+      </c>
+      <c r="F19">
+        <v>11200</v>
+      </c>
+      <c r="G19">
+        <v>370</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20">
+        <v>217</v>
+      </c>
+      <c r="B20" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20">
+        <v>28</v>
+      </c>
+      <c r="F20">
+        <v>10800</v>
+      </c>
+      <c r="G20">
+        <v>360</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <v>218</v>
+      </c>
+      <c r="B21" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>174</v>
+      </c>
+      <c r="E21">
+        <v>36</v>
+      </c>
+      <c r="F21">
+        <v>12300</v>
+      </c>
+      <c r="G21">
+        <v>390</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <v>219</v>
+      </c>
+      <c r="B22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>181</v>
+      </c>
+      <c r="E22">
+        <v>27</v>
+      </c>
+      <c r="F22">
+        <v>12600</v>
+      </c>
+      <c r="G22">
+        <v>360</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I22" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23">
+        <v>220</v>
+      </c>
+      <c r="B23" t="s">
+        <v>183</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>181</v>
+      </c>
+      <c r="E23">
+        <v>22</v>
+      </c>
+      <c r="F23">
+        <v>13600</v>
+      </c>
+      <c r="G23">
+        <v>350</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24">
+        <v>221</v>
+      </c>
+      <c r="B24" t="s">
+        <v>185</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>181</v>
+      </c>
+      <c r="E24">
+        <v>30</v>
+      </c>
+      <c r="F24">
+        <v>14600</v>
+      </c>
+      <c r="G24">
+        <v>380</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I24" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246DAC17-E872-4574-BD3D-D5CF034B9B32}">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="3" max="5" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>801</v>
+      </c>
+      <c r="B4">
+        <v>201</v>
+      </c>
+      <c r="C4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4">
+        <v>140</v>
+      </c>
+      <c r="G4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>802</v>
+      </c>
+      <c r="B5">
+        <v>202</v>
+      </c>
+      <c r="C5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F5">
+        <v>140</v>
+      </c>
+      <c r="G5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>803</v>
+      </c>
+      <c r="B6">
+        <v>203</v>
+      </c>
+      <c r="C6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F6">
+        <v>355</v>
+      </c>
+      <c r="G6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>804</v>
+      </c>
+      <c r="B7">
+        <v>204</v>
+      </c>
+      <c r="C7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7" t="s">
+        <v>198</v>
+      </c>
+      <c r="F7">
+        <v>355</v>
+      </c>
+      <c r="G7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>805</v>
+      </c>
+      <c r="B8">
+        <v>205</v>
+      </c>
+      <c r="C8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8">
+        <v>933</v>
+      </c>
+      <c r="G8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>806</v>
+      </c>
+      <c r="B9">
+        <v>206</v>
+      </c>
+      <c r="C9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F9">
+        <v>933</v>
+      </c>
+      <c r="G9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>807</v>
+      </c>
+      <c r="B10">
+        <v>207</v>
+      </c>
+      <c r="C10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10">
+        <v>140</v>
+      </c>
+      <c r="G10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>808</v>
+      </c>
+      <c r="B11">
+        <v>208</v>
+      </c>
+      <c r="C11" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E11" t="s">
+        <v>198</v>
+      </c>
+      <c r="F11">
+        <v>140</v>
+      </c>
+      <c r="G11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>809</v>
+      </c>
+      <c r="B12">
+        <v>209</v>
+      </c>
+      <c r="C12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" t="s">
+        <v>197</v>
+      </c>
+      <c r="E12" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12">
+        <v>355</v>
+      </c>
+      <c r="G12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>810</v>
+      </c>
+      <c r="B13">
+        <v>210</v>
+      </c>
+      <c r="C13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" t="s">
+        <v>197</v>
+      </c>
+      <c r="E13" t="s">
+        <v>198</v>
+      </c>
+      <c r="F13">
+        <v>355</v>
+      </c>
+      <c r="G13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>811</v>
+      </c>
+      <c r="B14">
+        <v>211</v>
+      </c>
+      <c r="C14" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" t="s">
+        <v>198</v>
+      </c>
+      <c r="F14">
+        <v>933</v>
+      </c>
+      <c r="G14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>812</v>
+      </c>
+      <c r="B15">
+        <v>212</v>
+      </c>
+      <c r="C15" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" t="s">
+        <v>197</v>
+      </c>
+      <c r="E15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F15">
+        <v>933</v>
+      </c>
+      <c r="G15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>813</v>
+      </c>
+      <c r="B16">
+        <v>213</v>
+      </c>
+      <c r="C16" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16" t="s">
+        <v>198</v>
+      </c>
+      <c r="F16">
+        <v>140</v>
+      </c>
+      <c r="G16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>814</v>
+      </c>
+      <c r="B17">
+        <v>214</v>
+      </c>
+      <c r="C17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17" t="s">
+        <v>197</v>
+      </c>
+      <c r="E17" t="s">
+        <v>198</v>
+      </c>
+      <c r="F17">
+        <v>140</v>
+      </c>
+      <c r="G17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>815</v>
+      </c>
+      <c r="B18">
+        <v>215</v>
+      </c>
+      <c r="C18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D18" t="s">
+        <v>197</v>
+      </c>
+      <c r="E18" t="s">
+        <v>198</v>
+      </c>
+      <c r="F18">
+        <v>140</v>
+      </c>
+      <c r="G18" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>816</v>
+      </c>
+      <c r="B19">
+        <v>216</v>
+      </c>
+      <c r="C19" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" t="s">
+        <v>198</v>
+      </c>
+      <c r="F19">
+        <v>355</v>
+      </c>
+      <c r="G19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>817</v>
+      </c>
+      <c r="B20">
+        <v>217</v>
+      </c>
+      <c r="C20" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" t="s">
+        <v>197</v>
+      </c>
+      <c r="E20" t="s">
+        <v>198</v>
+      </c>
+      <c r="F20">
+        <v>355</v>
+      </c>
+      <c r="G20" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>818</v>
+      </c>
+      <c r="B21">
+        <v>218</v>
+      </c>
+      <c r="C21" t="s">
+        <v>196</v>
+      </c>
+      <c r="D21" t="s">
+        <v>197</v>
+      </c>
+      <c r="E21" t="s">
+        <v>198</v>
+      </c>
+      <c r="F21">
+        <v>355</v>
+      </c>
+      <c r="G21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>819</v>
+      </c>
+      <c r="B22">
+        <v>219</v>
+      </c>
+      <c r="C22" t="s">
+        <v>196</v>
+      </c>
+      <c r="D22" t="s">
+        <v>197</v>
+      </c>
+      <c r="E22" t="s">
+        <v>198</v>
+      </c>
+      <c r="F22">
+        <v>933</v>
+      </c>
+      <c r="G22" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>820</v>
+      </c>
+      <c r="B23">
+        <v>220</v>
+      </c>
+      <c r="C23" t="s">
+        <v>196</v>
+      </c>
+      <c r="D23" t="s">
+        <v>197</v>
+      </c>
+      <c r="E23" t="s">
+        <v>198</v>
+      </c>
+      <c r="F23">
+        <v>933</v>
+      </c>
+      <c r="G23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>821</v>
+      </c>
+      <c r="B24">
+        <v>221</v>
+      </c>
+      <c r="C24" t="s">
+        <v>196</v>
+      </c>
+      <c r="D24" t="s">
+        <v>197</v>
+      </c>
+      <c r="E24" t="s">
+        <v>198</v>
+      </c>
+      <c r="F24">
+        <v>933</v>
+      </c>
+      <c r="G24" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Reapply "feat : UnitManager""
This reverts commit 878ff64532bff531c9780087d87207b25f533891.
</commit_message>
<xml_diff>
--- a/RawData/excel_files/DataTable.xlsx
+++ b/RawData/excel_files/DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grays\Desktop\Project\Unity\OIlNamProject\RawData\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C03177-41D9-4235-9C40-295C73EFD9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36379A7-9C58-4FE4-8CA0-65CA0BA0BF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34515" yWindow="1785" windowWidth="20010" windowHeight="11385" activeTab="6" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter" sheetId="4" r:id="rId1"/>
@@ -18,8 +18,6 @@
     <sheet name="Enemy" sheetId="1" r:id="rId3"/>
     <sheet name="Boss" sheetId="5" r:id="rId4"/>
     <sheet name="Message" sheetId="3" r:id="rId5"/>
-    <sheet name="Unit" sheetId="6" r:id="rId6"/>
-    <sheet name="Upgrade" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="132">
   <si>
     <t>Name</t>
   </si>
@@ -556,254 +554,6 @@
 인류는 멸망하지 않았다.
 균열에서 새어 나오는 마나를 받아들여
 특별한 힘을 지니게 된 사람들 덕분이었다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unit_Tier</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>ATK</t>
-  </si>
-  <si>
-    <t>Attack_Speed</t>
-  </si>
-  <si>
-    <t>Attack_Range</t>
-  </si>
-  <si>
-    <t>Unit_Modeling</t>
-  </si>
-  <si>
-    <t>가브리엘</t>
-  </si>
-  <si>
-    <t>세계를 구한 7대 영웅 중 1명입니다.</t>
-  </si>
-  <si>
-    <t>SS1_gif</t>
-  </si>
-  <si>
-    <t>잉그리드</t>
-  </si>
-  <si>
-    <t>SS2_gif</t>
-  </si>
-  <si>
-    <t>제이드</t>
-  </si>
-  <si>
-    <t>실력이 뛰어난 검사입니다.</t>
-  </si>
-  <si>
-    <t>SA3_gif</t>
-  </si>
-  <si>
-    <t>리</t>
-  </si>
-  <si>
-    <t>SA4_gif</t>
-  </si>
-  <si>
-    <t>잭슨</t>
-  </si>
-  <si>
-    <t>견습 검사입니다.</t>
-  </si>
-  <si>
-    <t>SB5_gif</t>
-  </si>
-  <si>
-    <t>잭</t>
-  </si>
-  <si>
-    <t>SB6_gif</t>
-  </si>
-  <si>
-    <t>칼리</t>
-  </si>
-  <si>
-    <t>AS1_gif</t>
-  </si>
-  <si>
-    <t>엘린</t>
-  </si>
-  <si>
-    <t>AS2_gif</t>
-  </si>
-  <si>
-    <t>체이스</t>
-  </si>
-  <si>
-    <t>실력이 뛰어난 궁수입니다.</t>
-  </si>
-  <si>
-    <t>AA3_gif</t>
-  </si>
-  <si>
-    <t>파벨</t>
-  </si>
-  <si>
-    <t>AA4_gif</t>
-  </si>
-  <si>
-    <t>매기</t>
-  </si>
-  <si>
-    <t>견습 궁수입니다.</t>
-  </si>
-  <si>
-    <t>AB5_gif</t>
-  </si>
-  <si>
-    <t>마돈나</t>
-  </si>
-  <si>
-    <t>AB6_gif</t>
-  </si>
-  <si>
-    <t>에반</t>
-  </si>
-  <si>
-    <t>WS1_gif</t>
-  </si>
-  <si>
-    <t>밤비</t>
-  </si>
-  <si>
-    <t>WS2_gif</t>
-  </si>
-  <si>
-    <t>오로라</t>
-  </si>
-  <si>
-    <t>WS3_gif</t>
-  </si>
-  <si>
-    <t>데이브</t>
-  </si>
-  <si>
-    <t>실력이 뛰어난 마법사입니다.</t>
-  </si>
-  <si>
-    <t>WA4_gif</t>
-  </si>
-  <si>
-    <t>데이지</t>
-  </si>
-  <si>
-    <t>WA5_gif</t>
-  </si>
-  <si>
-    <t>콜린</t>
-  </si>
-  <si>
-    <t>WA6_gif</t>
-  </si>
-  <si>
-    <t>아만다</t>
-  </si>
-  <si>
-    <t>견습 마법사입니다.</t>
-  </si>
-  <si>
-    <t>WB7_gif</t>
-  </si>
-  <si>
-    <t>오스카</t>
-  </si>
-  <si>
-    <t>WB8_gif</t>
-  </si>
-  <si>
-    <t>헤스티아</t>
-  </si>
-  <si>
-    <t>WB9_gif</t>
-  </si>
-  <si>
-    <t>Open</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>false</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>rue</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>UnitID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unit ID</t>
-  </si>
-  <si>
-    <t>Tier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ATK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12,23,34,45,56,67,78</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12,23,34,45,56,67,79</t>
-  </si>
-  <si>
-    <t>12,23,34,45,56,67,80</t>
-  </si>
-  <si>
-    <t>List&lt;int&gt;</t>
-  </si>
-  <si>
-    <t>List&lt;int&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Drop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NeedPiece</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1,2,3,4,5,6,7</t>
-  </si>
-  <si>
-    <t>1,2,3,4,5,6,7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -970,7 +720,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1033,9 +783,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3550,7 +3297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8FABB6-B12D-4D0B-ADBA-E809D3A5F66E}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -3748,7 +3495,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4213,7 +3960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40025AE-C7D8-4357-9319-EFD6B75D65B3}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
@@ -4756,1298 +4503,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3B3B7E-BA51-4E15-824F-73A2BFC53D10}">
-  <dimension ref="A1:I24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <cols>
-    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H1" t="s">
-        <v>187</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F3" t="s">
-        <v>135</v>
-      </c>
-      <c r="G3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="I3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4">
-        <v>201</v>
-      </c>
-      <c r="B4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E4">
-        <v>43</v>
-      </c>
-      <c r="F4">
-        <v>9500</v>
-      </c>
-      <c r="G4">
-        <v>280</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="I4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5">
-        <v>202</v>
-      </c>
-      <c r="B5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5">
-        <v>37</v>
-      </c>
-      <c r="F5">
-        <v>8700</v>
-      </c>
-      <c r="G5">
-        <v>280</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="I5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6">
-        <v>203</v>
-      </c>
-      <c r="B6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6">
-        <v>32</v>
-      </c>
-      <c r="F6">
-        <v>10600</v>
-      </c>
-      <c r="G6">
-        <v>260</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="I6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7">
-        <v>204</v>
-      </c>
-      <c r="B7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E7">
-        <v>26</v>
-      </c>
-      <c r="F7">
-        <v>9800</v>
-      </c>
-      <c r="G7">
-        <v>260</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8">
-        <v>205</v>
-      </c>
-      <c r="B8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>149</v>
-      </c>
-      <c r="E8">
-        <v>20</v>
-      </c>
-      <c r="F8">
-        <v>13000</v>
-      </c>
-      <c r="G8">
-        <v>240</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9">
-        <v>206</v>
-      </c>
-      <c r="B9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E9">
-        <v>14</v>
-      </c>
-      <c r="F9">
-        <v>12000</v>
-      </c>
-      <c r="G9">
-        <v>240</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10">
-        <v>207</v>
-      </c>
-      <c r="B10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>139</v>
-      </c>
-      <c r="E10">
-        <v>22</v>
-      </c>
-      <c r="F10">
-        <v>5200</v>
-      </c>
-      <c r="G10">
-        <v>350</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11">
-        <v>208</v>
-      </c>
-      <c r="B11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>139</v>
-      </c>
-      <c r="E11">
-        <v>18</v>
-      </c>
-      <c r="F11">
-        <v>4300</v>
-      </c>
-      <c r="G11">
-        <v>350</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12">
-        <v>209</v>
-      </c>
-      <c r="B12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>158</v>
-      </c>
-      <c r="E12">
-        <v>18</v>
-      </c>
-      <c r="F12">
-        <v>6300</v>
-      </c>
-      <c r="G12">
-        <v>320</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13">
-        <v>210</v>
-      </c>
-      <c r="B13" t="s">
-        <v>160</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>158</v>
-      </c>
-      <c r="E13">
-        <v>15</v>
-      </c>
-      <c r="F13">
-        <v>5600</v>
-      </c>
-      <c r="G13">
-        <v>320</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14">
-        <v>211</v>
-      </c>
-      <c r="B14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>163</v>
-      </c>
-      <c r="E14">
-        <v>17</v>
-      </c>
-      <c r="F14">
-        <v>7200</v>
-      </c>
-      <c r="G14">
-        <v>300</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I14" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15">
-        <v>212</v>
-      </c>
-      <c r="B15" t="s">
-        <v>165</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15" t="s">
-        <v>163</v>
-      </c>
-      <c r="E15">
-        <v>14</v>
-      </c>
-      <c r="F15">
-        <v>7800</v>
-      </c>
-      <c r="G15">
-        <v>300</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16">
-        <v>213</v>
-      </c>
-      <c r="B16" t="s">
-        <v>167</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>139</v>
-      </c>
-      <c r="E16">
-        <v>45</v>
-      </c>
-      <c r="F16">
-        <v>10300</v>
-      </c>
-      <c r="G16">
-        <v>410</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I16" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17">
-        <v>214</v>
-      </c>
-      <c r="B17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>139</v>
-      </c>
-      <c r="E17">
-        <v>40</v>
-      </c>
-      <c r="F17">
-        <v>9900</v>
-      </c>
-      <c r="G17">
-        <v>400</v>
-      </c>
-      <c r="H17" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I17" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18">
-        <v>215</v>
-      </c>
-      <c r="B18" t="s">
-        <v>171</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>139</v>
-      </c>
-      <c r="E18">
-        <v>48</v>
-      </c>
-      <c r="F18">
-        <v>12400</v>
-      </c>
-      <c r="G18">
-        <v>430</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19">
-        <v>216</v>
-      </c>
-      <c r="B19" t="s">
-        <v>173</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>174</v>
-      </c>
-      <c r="E19">
-        <v>33</v>
-      </c>
-      <c r="F19">
-        <v>11200</v>
-      </c>
-      <c r="G19">
-        <v>370</v>
-      </c>
-      <c r="H19" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I19" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20">
-        <v>217</v>
-      </c>
-      <c r="B20" t="s">
-        <v>176</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>174</v>
-      </c>
-      <c r="E20">
-        <v>28</v>
-      </c>
-      <c r="F20">
-        <v>10800</v>
-      </c>
-      <c r="G20">
-        <v>360</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I20" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21">
-        <v>218</v>
-      </c>
-      <c r="B21" t="s">
-        <v>178</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>174</v>
-      </c>
-      <c r="E21">
-        <v>36</v>
-      </c>
-      <c r="F21">
-        <v>12300</v>
-      </c>
-      <c r="G21">
-        <v>390</v>
-      </c>
-      <c r="H21" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I21" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22">
-        <v>219</v>
-      </c>
-      <c r="B22" t="s">
-        <v>180</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22" t="s">
-        <v>181</v>
-      </c>
-      <c r="E22">
-        <v>27</v>
-      </c>
-      <c r="F22">
-        <v>12600</v>
-      </c>
-      <c r="G22">
-        <v>360</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I22" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23">
-        <v>220</v>
-      </c>
-      <c r="B23" t="s">
-        <v>183</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23" t="s">
-        <v>181</v>
-      </c>
-      <c r="E23">
-        <v>22</v>
-      </c>
-      <c r="F23">
-        <v>13600</v>
-      </c>
-      <c r="G23">
-        <v>350</v>
-      </c>
-      <c r="H23" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I23" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24">
-        <v>221</v>
-      </c>
-      <c r="B24" t="s">
-        <v>185</v>
-      </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-      <c r="D24" t="s">
-        <v>181</v>
-      </c>
-      <c r="E24">
-        <v>30</v>
-      </c>
-      <c r="F24">
-        <v>14600</v>
-      </c>
-      <c r="G24">
-        <v>380</v>
-      </c>
-      <c r="H24" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="I24" t="s">
-        <v>186</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246DAC17-E872-4574-BD3D-D5CF034B9B32}">
-  <dimension ref="A1:G24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <cols>
-    <col min="3" max="5" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>195</v>
-      </c>
-      <c r="F1" t="s">
-        <v>201</v>
-      </c>
-      <c r="G1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E2" t="s">
-        <v>200</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>202</v>
-      </c>
-      <c r="G3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
-        <v>801</v>
-      </c>
-      <c r="B4">
-        <v>201</v>
-      </c>
-      <c r="C4" t="s">
-        <v>196</v>
-      </c>
-      <c r="D4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E4" t="s">
-        <v>198</v>
-      </c>
-      <c r="F4">
-        <v>140</v>
-      </c>
-      <c r="G4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>802</v>
-      </c>
-      <c r="B5">
-        <v>202</v>
-      </c>
-      <c r="C5" t="s">
-        <v>196</v>
-      </c>
-      <c r="D5" t="s">
-        <v>197</v>
-      </c>
-      <c r="E5" t="s">
-        <v>198</v>
-      </c>
-      <c r="F5">
-        <v>140</v>
-      </c>
-      <c r="G5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>803</v>
-      </c>
-      <c r="B6">
-        <v>203</v>
-      </c>
-      <c r="C6" t="s">
-        <v>196</v>
-      </c>
-      <c r="D6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F6">
-        <v>355</v>
-      </c>
-      <c r="G6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>804</v>
-      </c>
-      <c r="B7">
-        <v>204</v>
-      </c>
-      <c r="C7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D7" t="s">
-        <v>197</v>
-      </c>
-      <c r="E7" t="s">
-        <v>198</v>
-      </c>
-      <c r="F7">
-        <v>355</v>
-      </c>
-      <c r="G7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
-        <v>805</v>
-      </c>
-      <c r="B8">
-        <v>205</v>
-      </c>
-      <c r="C8" t="s">
-        <v>196</v>
-      </c>
-      <c r="D8" t="s">
-        <v>197</v>
-      </c>
-      <c r="E8" t="s">
-        <v>198</v>
-      </c>
-      <c r="F8">
-        <v>933</v>
-      </c>
-      <c r="G8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>806</v>
-      </c>
-      <c r="B9">
-        <v>206</v>
-      </c>
-      <c r="C9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" t="s">
-        <v>197</v>
-      </c>
-      <c r="E9" t="s">
-        <v>198</v>
-      </c>
-      <c r="F9">
-        <v>933</v>
-      </c>
-      <c r="G9" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <v>807</v>
-      </c>
-      <c r="B10">
-        <v>207</v>
-      </c>
-      <c r="C10" t="s">
-        <v>196</v>
-      </c>
-      <c r="D10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E10" t="s">
-        <v>198</v>
-      </c>
-      <c r="F10">
-        <v>140</v>
-      </c>
-      <c r="G10" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
-        <v>808</v>
-      </c>
-      <c r="B11">
-        <v>208</v>
-      </c>
-      <c r="C11" t="s">
-        <v>196</v>
-      </c>
-      <c r="D11" t="s">
-        <v>197</v>
-      </c>
-      <c r="E11" t="s">
-        <v>198</v>
-      </c>
-      <c r="F11">
-        <v>140</v>
-      </c>
-      <c r="G11" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
-        <v>809</v>
-      </c>
-      <c r="B12">
-        <v>209</v>
-      </c>
-      <c r="C12" t="s">
-        <v>196</v>
-      </c>
-      <c r="D12" t="s">
-        <v>197</v>
-      </c>
-      <c r="E12" t="s">
-        <v>198</v>
-      </c>
-      <c r="F12">
-        <v>355</v>
-      </c>
-      <c r="G12" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
-        <v>810</v>
-      </c>
-      <c r="B13">
-        <v>210</v>
-      </c>
-      <c r="C13" t="s">
-        <v>196</v>
-      </c>
-      <c r="D13" t="s">
-        <v>197</v>
-      </c>
-      <c r="E13" t="s">
-        <v>198</v>
-      </c>
-      <c r="F13">
-        <v>355</v>
-      </c>
-      <c r="G13" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
-        <v>811</v>
-      </c>
-      <c r="B14">
-        <v>211</v>
-      </c>
-      <c r="C14" t="s">
-        <v>196</v>
-      </c>
-      <c r="D14" t="s">
-        <v>197</v>
-      </c>
-      <c r="E14" t="s">
-        <v>198</v>
-      </c>
-      <c r="F14">
-        <v>933</v>
-      </c>
-      <c r="G14" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15">
-        <v>812</v>
-      </c>
-      <c r="B15">
-        <v>212</v>
-      </c>
-      <c r="C15" t="s">
-        <v>196</v>
-      </c>
-      <c r="D15" t="s">
-        <v>197</v>
-      </c>
-      <c r="E15" t="s">
-        <v>198</v>
-      </c>
-      <c r="F15">
-        <v>933</v>
-      </c>
-      <c r="G15" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16">
-        <v>813</v>
-      </c>
-      <c r="B16">
-        <v>213</v>
-      </c>
-      <c r="C16" t="s">
-        <v>196</v>
-      </c>
-      <c r="D16" t="s">
-        <v>197</v>
-      </c>
-      <c r="E16" t="s">
-        <v>198</v>
-      </c>
-      <c r="F16">
-        <v>140</v>
-      </c>
-      <c r="G16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17">
-        <v>814</v>
-      </c>
-      <c r="B17">
-        <v>214</v>
-      </c>
-      <c r="C17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D17" t="s">
-        <v>197</v>
-      </c>
-      <c r="E17" t="s">
-        <v>198</v>
-      </c>
-      <c r="F17">
-        <v>140</v>
-      </c>
-      <c r="G17" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18">
-        <v>815</v>
-      </c>
-      <c r="B18">
-        <v>215</v>
-      </c>
-      <c r="C18" t="s">
-        <v>196</v>
-      </c>
-      <c r="D18" t="s">
-        <v>197</v>
-      </c>
-      <c r="E18" t="s">
-        <v>198</v>
-      </c>
-      <c r="F18">
-        <v>140</v>
-      </c>
-      <c r="G18" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19">
-        <v>816</v>
-      </c>
-      <c r="B19">
-        <v>216</v>
-      </c>
-      <c r="C19" t="s">
-        <v>196</v>
-      </c>
-      <c r="D19" t="s">
-        <v>197</v>
-      </c>
-      <c r="E19" t="s">
-        <v>198</v>
-      </c>
-      <c r="F19">
-        <v>355</v>
-      </c>
-      <c r="G19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20">
-        <v>817</v>
-      </c>
-      <c r="B20">
-        <v>217</v>
-      </c>
-      <c r="C20" t="s">
-        <v>196</v>
-      </c>
-      <c r="D20" t="s">
-        <v>197</v>
-      </c>
-      <c r="E20" t="s">
-        <v>198</v>
-      </c>
-      <c r="F20">
-        <v>355</v>
-      </c>
-      <c r="G20" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21">
-        <v>818</v>
-      </c>
-      <c r="B21">
-        <v>218</v>
-      </c>
-      <c r="C21" t="s">
-        <v>196</v>
-      </c>
-      <c r="D21" t="s">
-        <v>197</v>
-      </c>
-      <c r="E21" t="s">
-        <v>198</v>
-      </c>
-      <c r="F21">
-        <v>355</v>
-      </c>
-      <c r="G21" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22">
-        <v>819</v>
-      </c>
-      <c r="B22">
-        <v>219</v>
-      </c>
-      <c r="C22" t="s">
-        <v>196</v>
-      </c>
-      <c r="D22" t="s">
-        <v>197</v>
-      </c>
-      <c r="E22" t="s">
-        <v>198</v>
-      </c>
-      <c r="F22">
-        <v>933</v>
-      </c>
-      <c r="G22" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23">
-        <v>820</v>
-      </c>
-      <c r="B23">
-        <v>220</v>
-      </c>
-      <c r="C23" t="s">
-        <v>196</v>
-      </c>
-      <c r="D23" t="s">
-        <v>197</v>
-      </c>
-      <c r="E23" t="s">
-        <v>198</v>
-      </c>
-      <c r="F23">
-        <v>933</v>
-      </c>
-      <c r="G23" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24">
-        <v>821</v>
-      </c>
-      <c r="B24">
-        <v>221</v>
-      </c>
-      <c r="C24" t="s">
-        <v>196</v>
-      </c>
-      <c r="D24" t="s">
-        <v>197</v>
-      </c>
-      <c r="E24" t="s">
-        <v>198</v>
-      </c>
-      <c r="F24">
-        <v>933</v>
-      </c>
-      <c r="G24" t="s">
-        <v>204</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Reapply "Reapply "feat : UnitManager""
This reverts commit 151183b7f5ca5f7cfeeddff57d271ef180b4eb6c.
</commit_message>
<xml_diff>
--- a/RawData/excel_files/DataTable.xlsx
+++ b/RawData/excel_files/DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grays\Desktop\Project\Unity\OIlNamProject\RawData\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36379A7-9C58-4FE4-8CA0-65CA0BA0BF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C03177-41D9-4235-9C40-295C73EFD9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
+    <workbookView xWindow="34515" yWindow="1785" windowWidth="20010" windowHeight="11385" activeTab="6" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Enemy" sheetId="1" r:id="rId3"/>
     <sheet name="Boss" sheetId="5" r:id="rId4"/>
     <sheet name="Message" sheetId="3" r:id="rId5"/>
+    <sheet name="Unit" sheetId="6" r:id="rId6"/>
+    <sheet name="Upgrade" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="206">
   <si>
     <t>Name</t>
   </si>
@@ -554,6 +556,254 @@
 인류는 멸망하지 않았다.
 균열에서 새어 나오는 마나를 받아들여
 특별한 힘을 지니게 된 사람들 덕분이었다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit_Tier</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ATK</t>
+  </si>
+  <si>
+    <t>Attack_Speed</t>
+  </si>
+  <si>
+    <t>Attack_Range</t>
+  </si>
+  <si>
+    <t>Unit_Modeling</t>
+  </si>
+  <si>
+    <t>가브리엘</t>
+  </si>
+  <si>
+    <t>세계를 구한 7대 영웅 중 1명입니다.</t>
+  </si>
+  <si>
+    <t>SS1_gif</t>
+  </si>
+  <si>
+    <t>잉그리드</t>
+  </si>
+  <si>
+    <t>SS2_gif</t>
+  </si>
+  <si>
+    <t>제이드</t>
+  </si>
+  <si>
+    <t>실력이 뛰어난 검사입니다.</t>
+  </si>
+  <si>
+    <t>SA3_gif</t>
+  </si>
+  <si>
+    <t>리</t>
+  </si>
+  <si>
+    <t>SA4_gif</t>
+  </si>
+  <si>
+    <t>잭슨</t>
+  </si>
+  <si>
+    <t>견습 검사입니다.</t>
+  </si>
+  <si>
+    <t>SB5_gif</t>
+  </si>
+  <si>
+    <t>잭</t>
+  </si>
+  <si>
+    <t>SB6_gif</t>
+  </si>
+  <si>
+    <t>칼리</t>
+  </si>
+  <si>
+    <t>AS1_gif</t>
+  </si>
+  <si>
+    <t>엘린</t>
+  </si>
+  <si>
+    <t>AS2_gif</t>
+  </si>
+  <si>
+    <t>체이스</t>
+  </si>
+  <si>
+    <t>실력이 뛰어난 궁수입니다.</t>
+  </si>
+  <si>
+    <t>AA3_gif</t>
+  </si>
+  <si>
+    <t>파벨</t>
+  </si>
+  <si>
+    <t>AA4_gif</t>
+  </si>
+  <si>
+    <t>매기</t>
+  </si>
+  <si>
+    <t>견습 궁수입니다.</t>
+  </si>
+  <si>
+    <t>AB5_gif</t>
+  </si>
+  <si>
+    <t>마돈나</t>
+  </si>
+  <si>
+    <t>AB6_gif</t>
+  </si>
+  <si>
+    <t>에반</t>
+  </si>
+  <si>
+    <t>WS1_gif</t>
+  </si>
+  <si>
+    <t>밤비</t>
+  </si>
+  <si>
+    <t>WS2_gif</t>
+  </si>
+  <si>
+    <t>오로라</t>
+  </si>
+  <si>
+    <t>WS3_gif</t>
+  </si>
+  <si>
+    <t>데이브</t>
+  </si>
+  <si>
+    <t>실력이 뛰어난 마법사입니다.</t>
+  </si>
+  <si>
+    <t>WA4_gif</t>
+  </si>
+  <si>
+    <t>데이지</t>
+  </si>
+  <si>
+    <t>WA5_gif</t>
+  </si>
+  <si>
+    <t>콜린</t>
+  </si>
+  <si>
+    <t>WA6_gif</t>
+  </si>
+  <si>
+    <t>아만다</t>
+  </si>
+  <si>
+    <t>견습 마법사입니다.</t>
+  </si>
+  <si>
+    <t>WB7_gif</t>
+  </si>
+  <si>
+    <t>오스카</t>
+  </si>
+  <si>
+    <t>WB8_gif</t>
+  </si>
+  <si>
+    <t>헤스티아</t>
+  </si>
+  <si>
+    <t>WB9_gif</t>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>rue</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UnitID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit ID</t>
+  </si>
+  <si>
+    <t>Tier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12,23,34,45,56,67,78</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12,23,34,45,56,67,79</t>
+  </si>
+  <si>
+    <t>12,23,34,45,56,67,80</t>
+  </si>
+  <si>
+    <t>List&lt;int&gt;</t>
+  </si>
+  <si>
+    <t>List&lt;int&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Drop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeedPiece</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -720,7 +970,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -783,6 +1033,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3297,7 +3550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8FABB6-B12D-4D0B-ADBA-E809D3A5F66E}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -3495,7 +3748,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3960,7 +4213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40025AE-C7D8-4357-9319-EFD6B75D65B3}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
@@ -4503,4 +4756,1298 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3B3B7E-BA51-4E15-824F-73A2BFC53D10}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>201</v>
+      </c>
+      <c r="B4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4">
+        <v>43</v>
+      </c>
+      <c r="F4">
+        <v>9500</v>
+      </c>
+      <c r="G4">
+        <v>280</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="I4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>202</v>
+      </c>
+      <c r="B5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5">
+        <v>37</v>
+      </c>
+      <c r="F5">
+        <v>8700</v>
+      </c>
+      <c r="G5">
+        <v>280</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="I5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>203</v>
+      </c>
+      <c r="B6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6">
+        <v>32</v>
+      </c>
+      <c r="F6">
+        <v>10600</v>
+      </c>
+      <c r="G6">
+        <v>260</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="I6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>204</v>
+      </c>
+      <c r="B7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7">
+        <v>26</v>
+      </c>
+      <c r="F7">
+        <v>9800</v>
+      </c>
+      <c r="G7">
+        <v>260</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>205</v>
+      </c>
+      <c r="B8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>13000</v>
+      </c>
+      <c r="G8">
+        <v>240</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>206</v>
+      </c>
+      <c r="B9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>12000</v>
+      </c>
+      <c r="G9">
+        <v>240</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>207</v>
+      </c>
+      <c r="B10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10">
+        <v>22</v>
+      </c>
+      <c r="F10">
+        <v>5200</v>
+      </c>
+      <c r="G10">
+        <v>350</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>208</v>
+      </c>
+      <c r="B11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11">
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <v>4300</v>
+      </c>
+      <c r="G11">
+        <v>350</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>209</v>
+      </c>
+      <c r="B12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12">
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>6300</v>
+      </c>
+      <c r="G12">
+        <v>320</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>210</v>
+      </c>
+      <c r="B13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>5600</v>
+      </c>
+      <c r="G13">
+        <v>320</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>211</v>
+      </c>
+      <c r="B14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14">
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>7200</v>
+      </c>
+      <c r="G14">
+        <v>300</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>212</v>
+      </c>
+      <c r="B15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="F15">
+        <v>7800</v>
+      </c>
+      <c r="G15">
+        <v>300</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>213</v>
+      </c>
+      <c r="B16" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16">
+        <v>45</v>
+      </c>
+      <c r="F16">
+        <v>10300</v>
+      </c>
+      <c r="G16">
+        <v>410</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>214</v>
+      </c>
+      <c r="B17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E17">
+        <v>40</v>
+      </c>
+      <c r="F17">
+        <v>9900</v>
+      </c>
+      <c r="G17">
+        <v>400</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18">
+        <v>215</v>
+      </c>
+      <c r="B18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>139</v>
+      </c>
+      <c r="E18">
+        <v>48</v>
+      </c>
+      <c r="F18">
+        <v>12400</v>
+      </c>
+      <c r="G18">
+        <v>430</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19">
+        <v>216</v>
+      </c>
+      <c r="B19" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>174</v>
+      </c>
+      <c r="E19">
+        <v>33</v>
+      </c>
+      <c r="F19">
+        <v>11200</v>
+      </c>
+      <c r="G19">
+        <v>370</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20">
+        <v>217</v>
+      </c>
+      <c r="B20" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20">
+        <v>28</v>
+      </c>
+      <c r="F20">
+        <v>10800</v>
+      </c>
+      <c r="G20">
+        <v>360</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <v>218</v>
+      </c>
+      <c r="B21" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>174</v>
+      </c>
+      <c r="E21">
+        <v>36</v>
+      </c>
+      <c r="F21">
+        <v>12300</v>
+      </c>
+      <c r="G21">
+        <v>390</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <v>219</v>
+      </c>
+      <c r="B22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>181</v>
+      </c>
+      <c r="E22">
+        <v>27</v>
+      </c>
+      <c r="F22">
+        <v>12600</v>
+      </c>
+      <c r="G22">
+        <v>360</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I22" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23">
+        <v>220</v>
+      </c>
+      <c r="B23" t="s">
+        <v>183</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>181</v>
+      </c>
+      <c r="E23">
+        <v>22</v>
+      </c>
+      <c r="F23">
+        <v>13600</v>
+      </c>
+      <c r="G23">
+        <v>350</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24">
+        <v>221</v>
+      </c>
+      <c r="B24" t="s">
+        <v>185</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>181</v>
+      </c>
+      <c r="E24">
+        <v>30</v>
+      </c>
+      <c r="F24">
+        <v>14600</v>
+      </c>
+      <c r="G24">
+        <v>380</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I24" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246DAC17-E872-4574-BD3D-D5CF034B9B32}">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="3" max="5" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>801</v>
+      </c>
+      <c r="B4">
+        <v>201</v>
+      </c>
+      <c r="C4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4">
+        <v>140</v>
+      </c>
+      <c r="G4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>802</v>
+      </c>
+      <c r="B5">
+        <v>202</v>
+      </c>
+      <c r="C5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F5">
+        <v>140</v>
+      </c>
+      <c r="G5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>803</v>
+      </c>
+      <c r="B6">
+        <v>203</v>
+      </c>
+      <c r="C6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F6">
+        <v>355</v>
+      </c>
+      <c r="G6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>804</v>
+      </c>
+      <c r="B7">
+        <v>204</v>
+      </c>
+      <c r="C7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7" t="s">
+        <v>198</v>
+      </c>
+      <c r="F7">
+        <v>355</v>
+      </c>
+      <c r="G7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>805</v>
+      </c>
+      <c r="B8">
+        <v>205</v>
+      </c>
+      <c r="C8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8">
+        <v>933</v>
+      </c>
+      <c r="G8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>806</v>
+      </c>
+      <c r="B9">
+        <v>206</v>
+      </c>
+      <c r="C9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F9">
+        <v>933</v>
+      </c>
+      <c r="G9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>807</v>
+      </c>
+      <c r="B10">
+        <v>207</v>
+      </c>
+      <c r="C10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10">
+        <v>140</v>
+      </c>
+      <c r="G10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>808</v>
+      </c>
+      <c r="B11">
+        <v>208</v>
+      </c>
+      <c r="C11" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E11" t="s">
+        <v>198</v>
+      </c>
+      <c r="F11">
+        <v>140</v>
+      </c>
+      <c r="G11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>809</v>
+      </c>
+      <c r="B12">
+        <v>209</v>
+      </c>
+      <c r="C12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" t="s">
+        <v>197</v>
+      </c>
+      <c r="E12" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12">
+        <v>355</v>
+      </c>
+      <c r="G12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>810</v>
+      </c>
+      <c r="B13">
+        <v>210</v>
+      </c>
+      <c r="C13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" t="s">
+        <v>197</v>
+      </c>
+      <c r="E13" t="s">
+        <v>198</v>
+      </c>
+      <c r="F13">
+        <v>355</v>
+      </c>
+      <c r="G13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>811</v>
+      </c>
+      <c r="B14">
+        <v>211</v>
+      </c>
+      <c r="C14" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" t="s">
+        <v>198</v>
+      </c>
+      <c r="F14">
+        <v>933</v>
+      </c>
+      <c r="G14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>812</v>
+      </c>
+      <c r="B15">
+        <v>212</v>
+      </c>
+      <c r="C15" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" t="s">
+        <v>197</v>
+      </c>
+      <c r="E15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F15">
+        <v>933</v>
+      </c>
+      <c r="G15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>813</v>
+      </c>
+      <c r="B16">
+        <v>213</v>
+      </c>
+      <c r="C16" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16" t="s">
+        <v>198</v>
+      </c>
+      <c r="F16">
+        <v>140</v>
+      </c>
+      <c r="G16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>814</v>
+      </c>
+      <c r="B17">
+        <v>214</v>
+      </c>
+      <c r="C17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17" t="s">
+        <v>197</v>
+      </c>
+      <c r="E17" t="s">
+        <v>198</v>
+      </c>
+      <c r="F17">
+        <v>140</v>
+      </c>
+      <c r="G17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>815</v>
+      </c>
+      <c r="B18">
+        <v>215</v>
+      </c>
+      <c r="C18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D18" t="s">
+        <v>197</v>
+      </c>
+      <c r="E18" t="s">
+        <v>198</v>
+      </c>
+      <c r="F18">
+        <v>140</v>
+      </c>
+      <c r="G18" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>816</v>
+      </c>
+      <c r="B19">
+        <v>216</v>
+      </c>
+      <c r="C19" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" t="s">
+        <v>198</v>
+      </c>
+      <c r="F19">
+        <v>355</v>
+      </c>
+      <c r="G19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>817</v>
+      </c>
+      <c r="B20">
+        <v>217</v>
+      </c>
+      <c r="C20" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" t="s">
+        <v>197</v>
+      </c>
+      <c r="E20" t="s">
+        <v>198</v>
+      </c>
+      <c r="F20">
+        <v>355</v>
+      </c>
+      <c r="G20" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>818</v>
+      </c>
+      <c r="B21">
+        <v>218</v>
+      </c>
+      <c r="C21" t="s">
+        <v>196</v>
+      </c>
+      <c r="D21" t="s">
+        <v>197</v>
+      </c>
+      <c r="E21" t="s">
+        <v>198</v>
+      </c>
+      <c r="F21">
+        <v>355</v>
+      </c>
+      <c r="G21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>819</v>
+      </c>
+      <c r="B22">
+        <v>219</v>
+      </c>
+      <c r="C22" t="s">
+        <v>196</v>
+      </c>
+      <c r="D22" t="s">
+        <v>197</v>
+      </c>
+      <c r="E22" t="s">
+        <v>198</v>
+      </c>
+      <c r="F22">
+        <v>933</v>
+      </c>
+      <c r="G22" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>820</v>
+      </c>
+      <c r="B23">
+        <v>220</v>
+      </c>
+      <c r="C23" t="s">
+        <v>196</v>
+      </c>
+      <c r="D23" t="s">
+        <v>197</v>
+      </c>
+      <c r="E23" t="s">
+        <v>198</v>
+      </c>
+      <c r="F23">
+        <v>933</v>
+      </c>
+      <c r="G23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>821</v>
+      </c>
+      <c r="B24">
+        <v>221</v>
+      </c>
+      <c r="C24" t="s">
+        <v>196</v>
+      </c>
+      <c r="D24" t="s">
+        <v>197</v>
+      </c>
+      <c r="E24" t="s">
+        <v>198</v>
+      </c>
+      <c r="F24">
+        <v>933</v>
+      </c>
+      <c r="G24" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat : 마물, 보스 animator controller 데이터 추가
</commit_message>
<xml_diff>
--- a/RawData/excel_files/DataTable.xlsx
+++ b/RawData/excel_files/DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grays\Desktop\Project\Unity\OIlNamProject\RawData\excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Portfolio\Oilnam\RawData\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DB3C99-5566-4DDE-9CCE-18E9DF00E294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCC6128-DD9E-4762-BA8C-1E4A19A8AD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33885" yWindow="1410" windowWidth="20010" windowHeight="11385" activeTab="5" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
+    <workbookView xWindow="930" yWindow="880" windowWidth="19200" windowHeight="11170" activeTab="2" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="234">
   <si>
     <t>Name</t>
   </si>
@@ -869,6 +869,62 @@
   <si>
     <t>AA2</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monster_Animatior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enemy/Enemy01Anim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enemy/Enemy03Anim</t>
+  </si>
+  <si>
+    <t>Enemy/Enemy04Anim</t>
+  </si>
+  <si>
+    <t>Enemy/Enemy05Anim</t>
+  </si>
+  <si>
+    <t>Enemy/Enemy06Anim</t>
+  </si>
+  <si>
+    <t>Enemy/Enemy07Anim</t>
+  </si>
+  <si>
+    <t>Enemy/Enemy08Anim</t>
+  </si>
+  <si>
+    <t>Enemy/Enemy09Anim</t>
+  </si>
+  <si>
+    <t>Enemy/Enemy10Anim</t>
+  </si>
+  <si>
+    <t>Enemy/Enemy02Anim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss/Boss01Anim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss/Boss03Anim</t>
+  </si>
+  <si>
+    <t>Boss/Boss04Anim</t>
+  </si>
+  <si>
+    <t>Boss/Boss05Anim</t>
+  </si>
+  <si>
+    <t>Boss/Boss02Anim</t>
   </si>
 </sst>
 </file>
@@ -1417,18 +1473,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AF03AA-AD2E-4842-8F07-034942C7A07E}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="5" max="6" width="11.625" customWidth="1"/>
-    <col min="8" max="8" width="14.875" customWidth="1"/>
+    <col min="5" max="6" width="11.58203125" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
     <col min="9" max="9" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="13.5" customWidth="1"/>
     <col min="11" max="11" width="18.75" customWidth="1"/>
-    <col min="12" max="12" width="10.875" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1513,7 +1569,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:13" ht="17.149999999999999" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -3607,6 +3663,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3618,10 +3675,10 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="2" max="2" width="104.875" customWidth="1"/>
-    <col min="3" max="3" width="7.125" customWidth="1"/>
+    <col min="2" max="2" width="104.83203125" customWidth="1"/>
+    <col min="3" max="3" width="7.08203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3668,7 +3725,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="49.5">
+    <row r="5" spans="1:3" ht="51">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3679,7 +3736,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="82.5">
+    <row r="6" spans="1:3" ht="85">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3690,7 +3747,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="82.5">
+    <row r="7" spans="1:3" ht="85">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3701,7 +3758,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="49.5">
+    <row r="8" spans="1:3" ht="51">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3712,7 +3769,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="82.5">
+    <row r="9" spans="1:3" ht="85">
       <c r="A9">
         <v>5</v>
       </c>
@@ -3723,7 +3780,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="66">
+    <row r="10" spans="1:3" ht="68">
       <c r="A10">
         <v>6</v>
       </c>
@@ -3734,7 +3791,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="49.5">
+    <row r="11" spans="1:3" ht="51">
       <c r="A11">
         <v>7</v>
       </c>
@@ -3745,7 +3802,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="66">
+    <row r="12" spans="1:3" ht="68">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3756,7 +3813,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="33">
+    <row r="13" spans="1:3" ht="34">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3767,7 +3824,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="115.5">
+    <row r="14" spans="1:3" ht="119">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3778,7 +3835,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="82.5">
+    <row r="15" spans="1:3" ht="85">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3809,22 +3866,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5409F1B1-0956-4B26-ACA9-55F5DBAB54F5}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="8.625" customWidth="1"/>
-    <col min="3" max="3" width="22.625" customWidth="1"/>
-    <col min="4" max="4" width="14.375" customWidth="1"/>
-    <col min="5" max="5" width="20.125" customWidth="1"/>
+    <col min="1" max="1" width="8.58203125" customWidth="1"/>
+    <col min="3" max="3" width="22.58203125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.08203125" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="19.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3843,8 +3901,11 @@
       <c r="F1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3863,8 +3924,11 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17.5" thickBot="1">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3883,8 +3947,11 @@
       <c r="F3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17.5" thickBot="1">
       <c r="A4" s="14">
         <v>401</v>
       </c>
@@ -3903,8 +3970,11 @@
       <c r="F4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17.5" thickBot="1">
       <c r="A5" s="16">
         <v>402</v>
       </c>
@@ -3923,8 +3993,11 @@
       <c r="F5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17.5" thickBot="1">
       <c r="A6" s="16">
         <v>403</v>
       </c>
@@ -3943,8 +4016,11 @@
       <c r="F6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17.5" thickBot="1">
       <c r="A7" s="16">
         <v>404</v>
       </c>
@@ -3963,8 +4039,11 @@
       <c r="F7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17.5" thickBot="1">
       <c r="A8" s="16">
         <v>405</v>
       </c>
@@ -3983,8 +4062,11 @@
       <c r="F8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17.5" thickBot="1">
       <c r="A9" s="16">
         <v>406</v>
       </c>
@@ -4003,8 +4085,11 @@
       <c r="F9" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17.5" thickBot="1">
       <c r="A10" s="16">
         <v>407</v>
       </c>
@@ -4023,8 +4108,11 @@
       <c r="F10" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17.5" thickBot="1">
       <c r="A11" s="16">
         <v>408</v>
       </c>
@@ -4043,8 +4131,11 @@
       <c r="F11" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G11" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17.5" thickBot="1">
       <c r="A12" s="16">
         <v>409</v>
       </c>
@@ -4063,8 +4154,11 @@
       <c r="F12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17.5" thickBot="1">
       <c r="A13" s="16">
         <v>410</v>
       </c>
@@ -4082,6 +4176,9 @@
       </c>
       <c r="F13" t="s">
         <v>86</v>
+      </c>
+      <c r="G13" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -4093,21 +4190,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B13BC7-908D-4893-B4AD-1079229E5F6F}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="3" max="3" width="16.375" customWidth="1"/>
-    <col min="4" max="4" width="14.375" customWidth="1"/>
-    <col min="5" max="5" width="20.625" customWidth="1"/>
-    <col min="6" max="6" width="13.625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.58203125" customWidth="1"/>
+    <col min="6" max="6" width="13.58203125" customWidth="1"/>
+    <col min="7" max="7" width="19.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -4126,8 +4224,11 @@
       <c r="F1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4146,8 +4247,11 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17.5" thickBot="1">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -4166,8 +4270,11 @@
       <c r="F3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17.5" thickBot="1">
       <c r="A4" s="14">
         <v>501</v>
       </c>
@@ -4186,8 +4293,11 @@
       <c r="F4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17.5" thickBot="1">
       <c r="A5" s="16">
         <v>502</v>
       </c>
@@ -4206,8 +4316,11 @@
       <c r="F5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17.5" thickBot="1">
       <c r="A6" s="16">
         <v>503</v>
       </c>
@@ -4226,8 +4339,11 @@
       <c r="F6" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17.5" thickBot="1">
       <c r="A7" s="16">
         <v>504</v>
       </c>
@@ -4246,8 +4362,11 @@
       <c r="F7" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17.5" thickBot="1">
       <c r="A8" s="16">
         <v>505</v>
       </c>
@@ -4265,11 +4384,15 @@
       </c>
       <c r="F8" t="s">
         <v>97</v>
+      </c>
+      <c r="G8" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4281,21 +4404,21 @@
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="8.625" customWidth="1"/>
-    <col min="2" max="2" width="31.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.58203125" customWidth="1"/>
+    <col min="2" max="2" width="31.58203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.58203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.08203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.58203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -4439,7 +4562,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="49.5">
+    <row r="4" spans="1:15" ht="51">
       <c r="A4">
         <v>3001</v>
       </c>
@@ -4486,7 +4609,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="49.5">
+    <row r="5" spans="1:15" ht="51">
       <c r="A5">
         <v>3002</v>
       </c>
@@ -4533,7 +4656,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="66">
+    <row r="6" spans="1:15" ht="68">
       <c r="A6">
         <v>3003</v>
       </c>
@@ -4580,7 +4703,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="49.5">
+    <row r="7" spans="1:15" ht="51">
       <c r="A7">
         <v>3004</v>
       </c>
@@ -4627,7 +4750,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="49.5">
+    <row r="8" spans="1:15" ht="51">
       <c r="A8">
         <v>3005</v>
       </c>
@@ -4674,7 +4797,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="49.5">
+    <row r="9" spans="1:15" ht="51">
       <c r="A9">
         <v>3006</v>
       </c>
@@ -4721,7 +4844,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="49.5">
+    <row r="10" spans="1:15" ht="51">
       <c r="A10">
         <v>3007</v>
       </c>
@@ -4768,7 +4891,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="49.5">
+    <row r="11" spans="1:15" ht="51">
       <c r="A11">
         <v>3008</v>
       </c>
@@ -4826,19 +4949,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3B3B7E-BA51-4E15-824F-73A2BFC53D10}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.08203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.58203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -5696,7 +5819,7 @@
       <selection activeCell="A4" sqref="A4:A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="37" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
feat : 골든패스 UI
</commit_message>
<xml_diff>
--- a/RawData/excel_files/DataTable.xlsx
+++ b/RawData/excel_files/DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Portfolio\Oilnam\RawData\excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grays\Desktop\Project\Unity\OIlNamProject\RawData\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3DBCCE-8341-4842-8F49-2C47020A8AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889AB647-51D0-4CD2-9E7A-43581CAB11FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2450" yWindow="1260" windowWidth="19200" windowHeight="11170" firstSheet="1" activeTab="9" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="12" xr2:uid="{FAA1F650-8D33-47ED-A566-792FFD777E9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter" sheetId="4" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Shop" sheetId="11" r:id="rId10"/>
     <sheet name="Goods" sheetId="12" r:id="rId11"/>
     <sheet name="TIP" sheetId="10" r:id="rId12"/>
+    <sheet name="LevelPass" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="361">
   <si>
     <t>Name</t>
   </si>
@@ -1343,6 +1344,42 @@
   </si>
   <si>
     <t>Is_Once</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LevelType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GoldenType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LevelValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GoldenValue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1929,14 +1966,14 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="5" max="6" width="11.58203125" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+    <col min="5" max="6" width="11.625" customWidth="1"/>
+    <col min="8" max="8" width="14.875" customWidth="1"/>
     <col min="9" max="9" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="13.5" customWidth="1"/>
     <col min="11" max="11" width="18.75" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" customWidth="1"/>
+    <col min="12" max="12" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2021,7 +2058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17.149999999999999" customHeight="1">
+    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -4123,26 +4160,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D50587-6B81-48DF-A8DB-00F001E27D99}">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" customWidth="1"/>
-    <col min="2" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="33.1640625" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="2" max="3" width="17.375" customWidth="1"/>
+    <col min="4" max="4" width="33.125" customWidth="1"/>
+    <col min="5" max="5" width="15.125" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="7" width="15.25" customWidth="1"/>
-    <col min="8" max="8" width="15.08203125" customWidth="1"/>
+    <col min="8" max="8" width="15.125" customWidth="1"/>
     <col min="9" max="9" width="15.75" customWidth="1"/>
     <col min="10" max="12" width="16" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
     <col min="14" max="14" width="14.25" customWidth="1"/>
-    <col min="15" max="16" width="14.83203125" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" customWidth="1"/>
-    <col min="18" max="18" width="14.83203125" customWidth="1"/>
+    <col min="15" max="16" width="14.875" customWidth="1"/>
+    <col min="17" max="17" width="13.625" customWidth="1"/>
+    <col min="18" max="18" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -5000,10 +5037,10 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="39.58203125" customWidth="1"/>
+    <col min="3" max="3" width="39.625" customWidth="1"/>
     <col min="4" max="4" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5021,7 +5058,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.5" thickBot="1">
+    <row r="2" spans="1:4" ht="17.25" thickBot="1">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5035,7 +5072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.5" thickBot="1">
+    <row r="3" spans="1:4" ht="17.25" thickBot="1">
       <c r="A3" s="23" t="s">
         <v>32</v>
       </c>
@@ -5049,7 +5086,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.5" thickBot="1">
+    <row r="4" spans="1:4" ht="17.25" thickBot="1">
       <c r="A4" s="16">
         <v>1501</v>
       </c>
@@ -5077,7 +5114,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="22" customHeight="1" thickBot="1">
+    <row r="6" spans="1:4" ht="21.95" customHeight="1" thickBot="1">
       <c r="A6" s="16">
         <v>1503</v>
       </c>
@@ -5091,7 +5128,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18.5" customHeight="1" thickBot="1">
+    <row r="7" spans="1:4" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A7" s="16">
         <v>1504</v>
       </c>
@@ -5105,7 +5142,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="21.5" customHeight="1" thickBot="1">
+    <row r="8" spans="1:4" ht="21.6" customHeight="1" thickBot="1">
       <c r="A8" s="16">
         <v>1505</v>
       </c>
@@ -5119,7 +5156,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22" customHeight="1" thickBot="1">
+    <row r="9" spans="1:4" ht="21.95" customHeight="1" thickBot="1">
       <c r="A9" s="16">
         <v>1506</v>
       </c>
@@ -5144,14 +5181,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6926D4-C54F-410A-A670-136E7C30B884}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="6.08203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5230,6 +5265,2737 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1FF4F24-FB0E-440A-9C75-674911EB633F}">
+  <dimension ref="A1:F145"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E1" t="s">
+        <v>359</v>
+      </c>
+      <c r="F1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E3" t="s">
+        <v>358</v>
+      </c>
+      <c r="F3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>10001</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>600</v>
+      </c>
+      <c r="F4" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>10002</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>200</v>
+      </c>
+      <c r="F5" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>10003</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>600</v>
+      </c>
+      <c r="F6" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>10004</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>200</v>
+      </c>
+      <c r="F7" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>10005</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>600</v>
+      </c>
+      <c r="F8" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>10006</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>200</v>
+      </c>
+      <c r="F9" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>10007</v>
+      </c>
+      <c r="B10" s="1">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>600</v>
+      </c>
+      <c r="F10" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>10008</v>
+      </c>
+      <c r="B11" s="1">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>600</v>
+      </c>
+      <c r="F11" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>10009</v>
+      </c>
+      <c r="B12" s="1">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>200</v>
+      </c>
+      <c r="F12" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>10010</v>
+      </c>
+      <c r="B13" s="1">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>600</v>
+      </c>
+      <c r="F13" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>10011</v>
+      </c>
+      <c r="B14" s="1">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>200</v>
+      </c>
+      <c r="F14" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>10012</v>
+      </c>
+      <c r="B15" s="1">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>600</v>
+      </c>
+      <c r="F15" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>10013</v>
+      </c>
+      <c r="B16" s="1">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1">
+        <v>200</v>
+      </c>
+      <c r="F16" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>10014</v>
+      </c>
+      <c r="B17" s="1">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>600</v>
+      </c>
+      <c r="F17" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>10015</v>
+      </c>
+      <c r="B18" s="1">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>600</v>
+      </c>
+      <c r="F18" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>10016</v>
+      </c>
+      <c r="B19" s="1">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>200</v>
+      </c>
+      <c r="F19" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>10017</v>
+      </c>
+      <c r="B20" s="1">
+        <v>17</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>600</v>
+      </c>
+      <c r="F20" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>10018</v>
+      </c>
+      <c r="B21" s="1">
+        <v>18</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>200</v>
+      </c>
+      <c r="F21" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>10019</v>
+      </c>
+      <c r="B22" s="1">
+        <v>19</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>600</v>
+      </c>
+      <c r="F22" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>10020</v>
+      </c>
+      <c r="B23" s="1">
+        <v>20</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1">
+        <v>200</v>
+      </c>
+      <c r="F23" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>10021</v>
+      </c>
+      <c r="B24" s="1">
+        <v>21</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1">
+        <v>600</v>
+      </c>
+      <c r="F24" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>10022</v>
+      </c>
+      <c r="B25" s="1">
+        <v>22</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>600</v>
+      </c>
+      <c r="F25" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1">
+        <v>10023</v>
+      </c>
+      <c r="B26" s="1">
+        <v>23</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>200</v>
+      </c>
+      <c r="F26" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1">
+        <v>10024</v>
+      </c>
+      <c r="B27" s="1">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>600</v>
+      </c>
+      <c r="F27" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1">
+        <v>10025</v>
+      </c>
+      <c r="B28" s="1">
+        <v>25</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1">
+        <v>200</v>
+      </c>
+      <c r="F28" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1">
+        <v>10026</v>
+      </c>
+      <c r="B29" s="1">
+        <v>26</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>600</v>
+      </c>
+      <c r="F29" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1">
+        <v>10027</v>
+      </c>
+      <c r="B30" s="1">
+        <v>27</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>200</v>
+      </c>
+      <c r="F30" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1">
+        <v>10028</v>
+      </c>
+      <c r="B31" s="1">
+        <v>28</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1">
+        <v>600</v>
+      </c>
+      <c r="F31" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1">
+        <v>10029</v>
+      </c>
+      <c r="B32" s="1">
+        <v>29</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>600</v>
+      </c>
+      <c r="F32" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1">
+        <v>10030</v>
+      </c>
+      <c r="B33" s="1">
+        <v>30</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1">
+        <v>200</v>
+      </c>
+      <c r="F33" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1">
+        <v>10031</v>
+      </c>
+      <c r="B34" s="1">
+        <v>31</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>600</v>
+      </c>
+      <c r="F34" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1">
+        <v>10032</v>
+      </c>
+      <c r="B35" s="1">
+        <v>32</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1">
+        <v>200</v>
+      </c>
+      <c r="F35" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1">
+        <v>10033</v>
+      </c>
+      <c r="B36" s="1">
+        <v>33</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1">
+        <v>600</v>
+      </c>
+      <c r="F36" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1">
+        <v>10034</v>
+      </c>
+      <c r="B37" s="1">
+        <v>34</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>200</v>
+      </c>
+      <c r="F37" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1">
+        <v>10035</v>
+      </c>
+      <c r="B38" s="1">
+        <v>35</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1">
+        <v>3</v>
+      </c>
+      <c r="E38" s="1">
+        <v>600</v>
+      </c>
+      <c r="F38" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1">
+        <v>10036</v>
+      </c>
+      <c r="B39" s="1">
+        <v>36</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1">
+        <v>600</v>
+      </c>
+      <c r="F39" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1">
+        <v>10037</v>
+      </c>
+      <c r="B40" s="1">
+        <v>37</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1">
+        <v>200</v>
+      </c>
+      <c r="F40" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1">
+        <v>10038</v>
+      </c>
+      <c r="B41" s="1">
+        <v>38</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>600</v>
+      </c>
+      <c r="F41" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="1">
+        <v>10039</v>
+      </c>
+      <c r="B42" s="1">
+        <v>39</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2</v>
+      </c>
+      <c r="E42" s="1">
+        <v>200</v>
+      </c>
+      <c r="F42" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="1">
+        <v>10040</v>
+      </c>
+      <c r="B43" s="1">
+        <v>40</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1">
+        <v>600</v>
+      </c>
+      <c r="F43" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="1">
+        <v>10041</v>
+      </c>
+      <c r="B44" s="1">
+        <v>41</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2</v>
+      </c>
+      <c r="E44" s="1">
+        <v>200</v>
+      </c>
+      <c r="F44" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="1">
+        <v>10042</v>
+      </c>
+      <c r="B45" s="1">
+        <v>42</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2</v>
+      </c>
+      <c r="D45" s="1">
+        <v>3</v>
+      </c>
+      <c r="E45" s="1">
+        <v>600</v>
+      </c>
+      <c r="F45" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="1">
+        <v>10043</v>
+      </c>
+      <c r="B46" s="1">
+        <v>43</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1">
+        <v>600</v>
+      </c>
+      <c r="F46" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="1">
+        <v>10044</v>
+      </c>
+      <c r="B47" s="1">
+        <v>44</v>
+      </c>
+      <c r="C47" s="1">
+        <v>2</v>
+      </c>
+      <c r="D47" s="1">
+        <v>2</v>
+      </c>
+      <c r="E47" s="1">
+        <v>200</v>
+      </c>
+      <c r="F47" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="1">
+        <v>10045</v>
+      </c>
+      <c r="B48" s="1">
+        <v>45</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1">
+        <v>600</v>
+      </c>
+      <c r="F48" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="1">
+        <v>10046</v>
+      </c>
+      <c r="B49" s="1">
+        <v>46</v>
+      </c>
+      <c r="C49" s="1">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1">
+        <v>2</v>
+      </c>
+      <c r="E49" s="1">
+        <v>200</v>
+      </c>
+      <c r="F49" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="1">
+        <v>10047</v>
+      </c>
+      <c r="B50" s="1">
+        <v>47</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1">
+        <v>600</v>
+      </c>
+      <c r="F50" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="1">
+        <v>10048</v>
+      </c>
+      <c r="B51" s="1">
+        <v>48</v>
+      </c>
+      <c r="C51" s="1">
+        <v>2</v>
+      </c>
+      <c r="D51" s="1">
+        <v>2</v>
+      </c>
+      <c r="E51" s="1">
+        <v>200</v>
+      </c>
+      <c r="F51" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="1">
+        <v>10049</v>
+      </c>
+      <c r="B52" s="1">
+        <v>49</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1">
+        <v>3</v>
+      </c>
+      <c r="E52" s="1">
+        <v>600</v>
+      </c>
+      <c r="F52" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="1">
+        <v>10050</v>
+      </c>
+      <c r="B53" s="1">
+        <v>50</v>
+      </c>
+      <c r="C53" s="1">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1</v>
+      </c>
+      <c r="E53" s="1">
+        <v>600</v>
+      </c>
+      <c r="F53" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="1">
+        <v>10051</v>
+      </c>
+      <c r="B54" s="1">
+        <v>51</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+      <c r="D54" s="1">
+        <v>2</v>
+      </c>
+      <c r="E54" s="1">
+        <v>200</v>
+      </c>
+      <c r="F54" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="1">
+        <v>10052</v>
+      </c>
+      <c r="B55" s="1">
+        <v>52</v>
+      </c>
+      <c r="C55" s="1">
+        <v>2</v>
+      </c>
+      <c r="D55" s="1">
+        <v>1</v>
+      </c>
+      <c r="E55" s="1">
+        <v>600</v>
+      </c>
+      <c r="F55" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="1">
+        <v>10053</v>
+      </c>
+      <c r="B56" s="1">
+        <v>53</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="1">
+        <v>2</v>
+      </c>
+      <c r="E56" s="1">
+        <v>200</v>
+      </c>
+      <c r="F56" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="1">
+        <v>10054</v>
+      </c>
+      <c r="B57" s="1">
+        <v>54</v>
+      </c>
+      <c r="C57" s="1">
+        <v>2</v>
+      </c>
+      <c r="D57" s="1">
+        <v>1</v>
+      </c>
+      <c r="E57" s="1">
+        <v>600</v>
+      </c>
+      <c r="F57" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="1">
+        <v>10055</v>
+      </c>
+      <c r="B58" s="1">
+        <v>55</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1</v>
+      </c>
+      <c r="D58" s="1">
+        <v>2</v>
+      </c>
+      <c r="E58" s="1">
+        <v>200</v>
+      </c>
+      <c r="F58" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="1">
+        <v>10056</v>
+      </c>
+      <c r="B59" s="1">
+        <v>56</v>
+      </c>
+      <c r="C59" s="1">
+        <v>2</v>
+      </c>
+      <c r="D59" s="1">
+        <v>3</v>
+      </c>
+      <c r="E59" s="1">
+        <v>600</v>
+      </c>
+      <c r="F59" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="1">
+        <v>10057</v>
+      </c>
+      <c r="B60" s="1">
+        <v>57</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1</v>
+      </c>
+      <c r="D60" s="1">
+        <v>1</v>
+      </c>
+      <c r="E60" s="1">
+        <v>600</v>
+      </c>
+      <c r="F60" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="1">
+        <v>10058</v>
+      </c>
+      <c r="B61" s="1">
+        <v>58</v>
+      </c>
+      <c r="C61" s="1">
+        <v>2</v>
+      </c>
+      <c r="D61" s="1">
+        <v>2</v>
+      </c>
+      <c r="E61" s="1">
+        <v>200</v>
+      </c>
+      <c r="F61" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="1">
+        <v>10059</v>
+      </c>
+      <c r="B62" s="1">
+        <v>59</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1</v>
+      </c>
+      <c r="D62" s="1">
+        <v>1</v>
+      </c>
+      <c r="E62" s="1">
+        <v>600</v>
+      </c>
+      <c r="F62" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="1">
+        <v>10060</v>
+      </c>
+      <c r="B63" s="1">
+        <v>60</v>
+      </c>
+      <c r="C63" s="1">
+        <v>2</v>
+      </c>
+      <c r="D63" s="1">
+        <v>2</v>
+      </c>
+      <c r="E63" s="1">
+        <v>200</v>
+      </c>
+      <c r="F63" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="1">
+        <v>10061</v>
+      </c>
+      <c r="B64" s="1">
+        <v>61</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1">
+        <v>1</v>
+      </c>
+      <c r="E64" s="1">
+        <v>600</v>
+      </c>
+      <c r="F64" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="1">
+        <v>10062</v>
+      </c>
+      <c r="B65" s="1">
+        <v>62</v>
+      </c>
+      <c r="C65" s="1">
+        <v>2</v>
+      </c>
+      <c r="D65" s="1">
+        <v>2</v>
+      </c>
+      <c r="E65" s="1">
+        <v>200</v>
+      </c>
+      <c r="F65" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="1">
+        <v>10063</v>
+      </c>
+      <c r="B66" s="1">
+        <v>63</v>
+      </c>
+      <c r="C66" s="1">
+        <v>1</v>
+      </c>
+      <c r="D66" s="1">
+        <v>3</v>
+      </c>
+      <c r="E66" s="1">
+        <v>600</v>
+      </c>
+      <c r="F66" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="1">
+        <v>10064</v>
+      </c>
+      <c r="B67" s="1">
+        <v>64</v>
+      </c>
+      <c r="C67" s="1">
+        <v>2</v>
+      </c>
+      <c r="D67" s="1">
+        <v>1</v>
+      </c>
+      <c r="E67" s="1">
+        <v>600</v>
+      </c>
+      <c r="F67" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="1">
+        <v>10065</v>
+      </c>
+      <c r="B68" s="1">
+        <v>65</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1</v>
+      </c>
+      <c r="D68" s="1">
+        <v>2</v>
+      </c>
+      <c r="E68" s="1">
+        <v>200</v>
+      </c>
+      <c r="F68" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="1">
+        <v>10066</v>
+      </c>
+      <c r="B69" s="1">
+        <v>66</v>
+      </c>
+      <c r="C69" s="1">
+        <v>2</v>
+      </c>
+      <c r="D69" s="1">
+        <v>1</v>
+      </c>
+      <c r="E69" s="1">
+        <v>600</v>
+      </c>
+      <c r="F69" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="1">
+        <v>10067</v>
+      </c>
+      <c r="B70" s="1">
+        <v>67</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+      <c r="D70" s="1">
+        <v>2</v>
+      </c>
+      <c r="E70" s="1">
+        <v>200</v>
+      </c>
+      <c r="F70" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="1">
+        <v>10068</v>
+      </c>
+      <c r="B71" s="1">
+        <v>68</v>
+      </c>
+      <c r="C71" s="1">
+        <v>2</v>
+      </c>
+      <c r="D71" s="1">
+        <v>1</v>
+      </c>
+      <c r="E71" s="1">
+        <v>600</v>
+      </c>
+      <c r="F71" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="1">
+        <v>10069</v>
+      </c>
+      <c r="B72" s="1">
+        <v>69</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1</v>
+      </c>
+      <c r="D72" s="1">
+        <v>2</v>
+      </c>
+      <c r="E72" s="1">
+        <v>200</v>
+      </c>
+      <c r="F72" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="1">
+        <v>10070</v>
+      </c>
+      <c r="B73" s="1">
+        <v>70</v>
+      </c>
+      <c r="C73" s="1">
+        <v>2</v>
+      </c>
+      <c r="D73" s="1">
+        <v>3</v>
+      </c>
+      <c r="E73" s="1">
+        <v>600</v>
+      </c>
+      <c r="F73" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="1">
+        <v>10071</v>
+      </c>
+      <c r="B74" s="1">
+        <v>71</v>
+      </c>
+      <c r="C74" s="1">
+        <v>1</v>
+      </c>
+      <c r="D74" s="1">
+        <v>1</v>
+      </c>
+      <c r="E74" s="1">
+        <v>200</v>
+      </c>
+      <c r="F74" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="1">
+        <v>10072</v>
+      </c>
+      <c r="B75" s="1">
+        <v>72</v>
+      </c>
+      <c r="C75" s="1">
+        <v>2</v>
+      </c>
+      <c r="D75" s="1">
+        <v>2</v>
+      </c>
+      <c r="E75" s="1">
+        <v>600</v>
+      </c>
+      <c r="F75" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="1">
+        <v>10073</v>
+      </c>
+      <c r="B76" s="1">
+        <v>73</v>
+      </c>
+      <c r="C76" s="1">
+        <v>1</v>
+      </c>
+      <c r="D76" s="1">
+        <v>1</v>
+      </c>
+      <c r="E76" s="1">
+        <v>200</v>
+      </c>
+      <c r="F76" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="1">
+        <v>10074</v>
+      </c>
+      <c r="B77" s="1">
+        <v>74</v>
+      </c>
+      <c r="C77" s="1">
+        <v>2</v>
+      </c>
+      <c r="D77" s="1">
+        <v>2</v>
+      </c>
+      <c r="E77" s="1">
+        <v>600</v>
+      </c>
+      <c r="F77" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="1">
+        <v>10075</v>
+      </c>
+      <c r="B78" s="1">
+        <v>75</v>
+      </c>
+      <c r="C78" s="1">
+        <v>1</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1</v>
+      </c>
+      <c r="E78" s="1">
+        <v>600</v>
+      </c>
+      <c r="F78" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="1">
+        <v>10076</v>
+      </c>
+      <c r="B79" s="1">
+        <v>76</v>
+      </c>
+      <c r="C79" s="1">
+        <v>2</v>
+      </c>
+      <c r="D79" s="1">
+        <v>2</v>
+      </c>
+      <c r="E79" s="1">
+        <v>200</v>
+      </c>
+      <c r="F79" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="1">
+        <v>10077</v>
+      </c>
+      <c r="B80" s="1">
+        <v>77</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1</v>
+      </c>
+      <c r="D80" s="1">
+        <v>3</v>
+      </c>
+      <c r="E80" s="1">
+        <v>600</v>
+      </c>
+      <c r="F80" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="1">
+        <v>10078</v>
+      </c>
+      <c r="B81" s="1">
+        <v>78</v>
+      </c>
+      <c r="C81" s="1">
+        <v>2</v>
+      </c>
+      <c r="D81" s="1">
+        <v>1</v>
+      </c>
+      <c r="E81" s="1">
+        <v>200</v>
+      </c>
+      <c r="F81" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="1">
+        <v>10079</v>
+      </c>
+      <c r="B82" s="1">
+        <v>79</v>
+      </c>
+      <c r="C82" s="1">
+        <v>1</v>
+      </c>
+      <c r="D82" s="1">
+        <v>2</v>
+      </c>
+      <c r="E82" s="1">
+        <v>600</v>
+      </c>
+      <c r="F82" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="1">
+        <v>10080</v>
+      </c>
+      <c r="B83" s="1">
+        <v>80</v>
+      </c>
+      <c r="C83" s="1">
+        <v>2</v>
+      </c>
+      <c r="D83" s="1">
+        <v>1</v>
+      </c>
+      <c r="E83" s="1">
+        <v>200</v>
+      </c>
+      <c r="F83" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="1">
+        <v>10081</v>
+      </c>
+      <c r="B84" s="1">
+        <v>81</v>
+      </c>
+      <c r="C84" s="1">
+        <v>1</v>
+      </c>
+      <c r="D84" s="1">
+        <v>2</v>
+      </c>
+      <c r="E84" s="1">
+        <v>600</v>
+      </c>
+      <c r="F84" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="1">
+        <v>10082</v>
+      </c>
+      <c r="B85" s="1">
+        <v>82</v>
+      </c>
+      <c r="C85" s="1">
+        <v>2</v>
+      </c>
+      <c r="D85" s="1">
+        <v>1</v>
+      </c>
+      <c r="E85" s="1">
+        <v>600</v>
+      </c>
+      <c r="F85" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="1">
+        <v>10083</v>
+      </c>
+      <c r="B86" s="1">
+        <v>83</v>
+      </c>
+      <c r="C86" s="1">
+        <v>1</v>
+      </c>
+      <c r="D86" s="1">
+        <v>2</v>
+      </c>
+      <c r="E86" s="1">
+        <v>200</v>
+      </c>
+      <c r="F86" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="1">
+        <v>10084</v>
+      </c>
+      <c r="B87" s="1">
+        <v>84</v>
+      </c>
+      <c r="C87" s="1">
+        <v>2</v>
+      </c>
+      <c r="D87" s="1">
+        <v>3</v>
+      </c>
+      <c r="E87" s="1">
+        <v>600</v>
+      </c>
+      <c r="F87" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="1">
+        <v>10085</v>
+      </c>
+      <c r="B88" s="1">
+        <v>85</v>
+      </c>
+      <c r="C88" s="1">
+        <v>1</v>
+      </c>
+      <c r="D88" s="1">
+        <v>1</v>
+      </c>
+      <c r="E88" s="1">
+        <v>200</v>
+      </c>
+      <c r="F88" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="1">
+        <v>10086</v>
+      </c>
+      <c r="B89" s="1">
+        <v>86</v>
+      </c>
+      <c r="C89" s="1">
+        <v>2</v>
+      </c>
+      <c r="D89" s="1">
+        <v>2</v>
+      </c>
+      <c r="E89" s="1">
+        <v>600</v>
+      </c>
+      <c r="F89" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="1">
+        <v>10087</v>
+      </c>
+      <c r="B90" s="1">
+        <v>87</v>
+      </c>
+      <c r="C90" s="1">
+        <v>1</v>
+      </c>
+      <c r="D90" s="1">
+        <v>1</v>
+      </c>
+      <c r="E90" s="1">
+        <v>200</v>
+      </c>
+      <c r="F90" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="1">
+        <v>10088</v>
+      </c>
+      <c r="B91" s="1">
+        <v>88</v>
+      </c>
+      <c r="C91" s="1">
+        <v>2</v>
+      </c>
+      <c r="D91" s="1">
+        <v>2</v>
+      </c>
+      <c r="E91" s="1">
+        <v>600</v>
+      </c>
+      <c r="F91" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="1">
+        <v>10089</v>
+      </c>
+      <c r="B92" s="1">
+        <v>89</v>
+      </c>
+      <c r="C92" s="1">
+        <v>1</v>
+      </c>
+      <c r="D92" s="1">
+        <v>1</v>
+      </c>
+      <c r="E92" s="1">
+        <v>200</v>
+      </c>
+      <c r="F92" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="1">
+        <v>10090</v>
+      </c>
+      <c r="B93" s="1">
+        <v>90</v>
+      </c>
+      <c r="C93" s="1">
+        <v>2</v>
+      </c>
+      <c r="D93" s="1">
+        <v>2</v>
+      </c>
+      <c r="E93" s="1">
+        <v>600</v>
+      </c>
+      <c r="F93" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="1">
+        <v>10091</v>
+      </c>
+      <c r="B94" s="1">
+        <v>91</v>
+      </c>
+      <c r="C94" s="1">
+        <v>1</v>
+      </c>
+      <c r="D94" s="1">
+        <v>3</v>
+      </c>
+      <c r="E94" s="1">
+        <v>200</v>
+      </c>
+      <c r="F94" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="1">
+        <v>10092</v>
+      </c>
+      <c r="B95" s="1">
+        <v>92</v>
+      </c>
+      <c r="C95" s="1">
+        <v>2</v>
+      </c>
+      <c r="D95" s="1">
+        <v>1</v>
+      </c>
+      <c r="E95" s="1">
+        <v>600</v>
+      </c>
+      <c r="F95" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="1">
+        <v>10093</v>
+      </c>
+      <c r="B96" s="1">
+        <v>93</v>
+      </c>
+      <c r="C96" s="1">
+        <v>1</v>
+      </c>
+      <c r="D96" s="1">
+        <v>2</v>
+      </c>
+      <c r="E96" s="1">
+        <v>600</v>
+      </c>
+      <c r="F96" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="1">
+        <v>10094</v>
+      </c>
+      <c r="B97" s="1">
+        <v>94</v>
+      </c>
+      <c r="C97" s="1">
+        <v>2</v>
+      </c>
+      <c r="D97" s="1">
+        <v>1</v>
+      </c>
+      <c r="E97" s="1">
+        <v>200</v>
+      </c>
+      <c r="F97" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="1">
+        <v>10095</v>
+      </c>
+      <c r="B98" s="1">
+        <v>95</v>
+      </c>
+      <c r="C98" s="1">
+        <v>1</v>
+      </c>
+      <c r="D98" s="1">
+        <v>2</v>
+      </c>
+      <c r="E98" s="1">
+        <v>600</v>
+      </c>
+      <c r="F98" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="1">
+        <v>10096</v>
+      </c>
+      <c r="B99" s="1">
+        <v>96</v>
+      </c>
+      <c r="C99" s="1">
+        <v>2</v>
+      </c>
+      <c r="D99" s="1">
+        <v>1</v>
+      </c>
+      <c r="E99" s="1">
+        <v>200</v>
+      </c>
+      <c r="F99" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="1">
+        <v>10097</v>
+      </c>
+      <c r="B100" s="1">
+        <v>97</v>
+      </c>
+      <c r="C100" s="1">
+        <v>1</v>
+      </c>
+      <c r="D100" s="1">
+        <v>2</v>
+      </c>
+      <c r="E100" s="1">
+        <v>600</v>
+      </c>
+      <c r="F100" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" s="1">
+        <v>10098</v>
+      </c>
+      <c r="B101" s="1">
+        <v>98</v>
+      </c>
+      <c r="C101" s="1">
+        <v>2</v>
+      </c>
+      <c r="D101" s="1">
+        <v>3</v>
+      </c>
+      <c r="E101" s="1">
+        <v>200</v>
+      </c>
+      <c r="F101" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="1">
+        <v>10099</v>
+      </c>
+      <c r="B102" s="1">
+        <v>99</v>
+      </c>
+      <c r="C102" s="1">
+        <v>1</v>
+      </c>
+      <c r="D102" s="1">
+        <v>1</v>
+      </c>
+      <c r="E102" s="1">
+        <v>600</v>
+      </c>
+      <c r="F102" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" s="1">
+        <v>10100</v>
+      </c>
+      <c r="B103" s="1">
+        <v>100</v>
+      </c>
+      <c r="C103" s="1">
+        <v>2</v>
+      </c>
+      <c r="D103" s="1">
+        <v>2</v>
+      </c>
+      <c r="E103" s="1">
+        <v>600</v>
+      </c>
+      <c r="F103" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="1">
+        <v>10101</v>
+      </c>
+      <c r="B104" s="1">
+        <v>101</v>
+      </c>
+      <c r="C104" s="1">
+        <v>1</v>
+      </c>
+      <c r="D104" s="1">
+        <v>1</v>
+      </c>
+      <c r="E104" s="1">
+        <v>200</v>
+      </c>
+      <c r="F104" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="1">
+        <v>10102</v>
+      </c>
+      <c r="B105" s="1">
+        <v>102</v>
+      </c>
+      <c r="C105" s="1">
+        <v>2</v>
+      </c>
+      <c r="D105" s="1">
+        <v>2</v>
+      </c>
+      <c r="E105" s="1">
+        <v>600</v>
+      </c>
+      <c r="F105" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="1">
+        <v>10103</v>
+      </c>
+      <c r="B106" s="1">
+        <v>103</v>
+      </c>
+      <c r="C106" s="1">
+        <v>1</v>
+      </c>
+      <c r="D106" s="1">
+        <v>1</v>
+      </c>
+      <c r="E106" s="1">
+        <v>200</v>
+      </c>
+      <c r="F106" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="1">
+        <v>10104</v>
+      </c>
+      <c r="B107" s="1">
+        <v>104</v>
+      </c>
+      <c r="C107" s="1">
+        <v>2</v>
+      </c>
+      <c r="D107" s="1">
+        <v>2</v>
+      </c>
+      <c r="E107" s="1">
+        <v>600</v>
+      </c>
+      <c r="F107" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="1">
+        <v>10105</v>
+      </c>
+      <c r="B108" s="1">
+        <v>105</v>
+      </c>
+      <c r="C108" s="1">
+        <v>1</v>
+      </c>
+      <c r="D108" s="1">
+        <v>3</v>
+      </c>
+      <c r="E108" s="1">
+        <v>200</v>
+      </c>
+      <c r="F108" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="1">
+        <v>10106</v>
+      </c>
+      <c r="B109" s="1">
+        <v>106</v>
+      </c>
+      <c r="C109" s="1">
+        <v>2</v>
+      </c>
+      <c r="D109" s="1">
+        <v>1</v>
+      </c>
+      <c r="E109" s="1">
+        <v>600</v>
+      </c>
+      <c r="F109" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="1">
+        <v>10107</v>
+      </c>
+      <c r="B110" s="1">
+        <v>107</v>
+      </c>
+      <c r="C110" s="1">
+        <v>1</v>
+      </c>
+      <c r="D110" s="1">
+        <v>2</v>
+      </c>
+      <c r="E110" s="1">
+        <v>200</v>
+      </c>
+      <c r="F110" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="1">
+        <v>10108</v>
+      </c>
+      <c r="B111" s="1">
+        <v>108</v>
+      </c>
+      <c r="C111" s="1">
+        <v>2</v>
+      </c>
+      <c r="D111" s="1">
+        <v>1</v>
+      </c>
+      <c r="E111" s="1">
+        <v>600</v>
+      </c>
+      <c r="F111" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" s="1">
+        <v>10109</v>
+      </c>
+      <c r="B112" s="1">
+        <v>109</v>
+      </c>
+      <c r="C112" s="1">
+        <v>1</v>
+      </c>
+      <c r="D112" s="1">
+        <v>2</v>
+      </c>
+      <c r="E112" s="1">
+        <v>200</v>
+      </c>
+      <c r="F112" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="1">
+        <v>10110</v>
+      </c>
+      <c r="B113" s="1">
+        <v>110</v>
+      </c>
+      <c r="C113" s="1">
+        <v>2</v>
+      </c>
+      <c r="D113" s="1">
+        <v>1</v>
+      </c>
+      <c r="E113" s="1">
+        <v>600</v>
+      </c>
+      <c r="F113" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" s="1">
+        <v>10111</v>
+      </c>
+      <c r="B114" s="1">
+        <v>111</v>
+      </c>
+      <c r="C114" s="1">
+        <v>1</v>
+      </c>
+      <c r="D114" s="1">
+        <v>2</v>
+      </c>
+      <c r="E114" s="1">
+        <v>600</v>
+      </c>
+      <c r="F114" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" s="1">
+        <v>10112</v>
+      </c>
+      <c r="B115" s="1">
+        <v>112</v>
+      </c>
+      <c r="C115" s="1">
+        <v>2</v>
+      </c>
+      <c r="D115" s="1">
+        <v>3</v>
+      </c>
+      <c r="E115" s="1">
+        <v>200</v>
+      </c>
+      <c r="F115" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" s="1">
+        <v>10113</v>
+      </c>
+      <c r="B116" s="1">
+        <v>113</v>
+      </c>
+      <c r="C116" s="1">
+        <v>1</v>
+      </c>
+      <c r="D116" s="1">
+        <v>1</v>
+      </c>
+      <c r="E116" s="1">
+        <v>600</v>
+      </c>
+      <c r="F116" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" s="1">
+        <v>10114</v>
+      </c>
+      <c r="B117" s="1">
+        <v>114</v>
+      </c>
+      <c r="C117" s="1">
+        <v>2</v>
+      </c>
+      <c r="D117" s="1">
+        <v>2</v>
+      </c>
+      <c r="E117" s="1">
+        <v>200</v>
+      </c>
+      <c r="F117" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" s="1">
+        <v>10115</v>
+      </c>
+      <c r="B118" s="1">
+        <v>115</v>
+      </c>
+      <c r="C118" s="1">
+        <v>1</v>
+      </c>
+      <c r="D118" s="1">
+        <v>1</v>
+      </c>
+      <c r="E118" s="1">
+        <v>600</v>
+      </c>
+      <c r="F118" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" s="1">
+        <v>10116</v>
+      </c>
+      <c r="B119" s="1">
+        <v>116</v>
+      </c>
+      <c r="C119" s="1">
+        <v>2</v>
+      </c>
+      <c r="D119" s="1">
+        <v>2</v>
+      </c>
+      <c r="E119" s="1">
+        <v>200</v>
+      </c>
+      <c r="F119" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120" s="1">
+        <v>10117</v>
+      </c>
+      <c r="B120" s="1">
+        <v>117</v>
+      </c>
+      <c r="C120" s="1">
+        <v>1</v>
+      </c>
+      <c r="D120" s="1">
+        <v>1</v>
+      </c>
+      <c r="E120" s="1">
+        <v>600</v>
+      </c>
+      <c r="F120" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="1">
+        <v>10118</v>
+      </c>
+      <c r="B121" s="1">
+        <v>118</v>
+      </c>
+      <c r="C121" s="1">
+        <v>2</v>
+      </c>
+      <c r="D121" s="1">
+        <v>2</v>
+      </c>
+      <c r="E121" s="1">
+        <v>600</v>
+      </c>
+      <c r="F121" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="1">
+        <v>10119</v>
+      </c>
+      <c r="B122" s="1">
+        <v>119</v>
+      </c>
+      <c r="C122" s="1">
+        <v>1</v>
+      </c>
+      <c r="D122" s="1">
+        <v>3</v>
+      </c>
+      <c r="E122" s="1">
+        <v>200</v>
+      </c>
+      <c r="F122" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="1">
+        <v>10120</v>
+      </c>
+      <c r="B123" s="1">
+        <v>120</v>
+      </c>
+      <c r="C123" s="1">
+        <v>2</v>
+      </c>
+      <c r="D123" s="1">
+        <v>1</v>
+      </c>
+      <c r="E123" s="1">
+        <v>600</v>
+      </c>
+      <c r="F123" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="1">
+        <v>10121</v>
+      </c>
+      <c r="B124" s="1">
+        <v>121</v>
+      </c>
+      <c r="C124" s="1">
+        <v>1</v>
+      </c>
+      <c r="D124" s="1">
+        <v>2</v>
+      </c>
+      <c r="E124" s="1">
+        <v>200</v>
+      </c>
+      <c r="F124" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" s="1">
+        <v>10122</v>
+      </c>
+      <c r="B125" s="1">
+        <v>122</v>
+      </c>
+      <c r="C125" s="1">
+        <v>2</v>
+      </c>
+      <c r="D125" s="1">
+        <v>1</v>
+      </c>
+      <c r="E125" s="1">
+        <v>600</v>
+      </c>
+      <c r="F125" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" s="1">
+        <v>10123</v>
+      </c>
+      <c r="B126" s="1">
+        <v>123</v>
+      </c>
+      <c r="C126" s="1">
+        <v>1</v>
+      </c>
+      <c r="D126" s="1">
+        <v>2</v>
+      </c>
+      <c r="E126" s="1">
+        <v>200</v>
+      </c>
+      <c r="F126" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" s="1">
+        <v>10124</v>
+      </c>
+      <c r="B127" s="1">
+        <v>124</v>
+      </c>
+      <c r="C127" s="1">
+        <v>2</v>
+      </c>
+      <c r="D127" s="1">
+        <v>1</v>
+      </c>
+      <c r="E127" s="1">
+        <v>600</v>
+      </c>
+      <c r="F127" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" s="1">
+        <v>10125</v>
+      </c>
+      <c r="B128" s="1">
+        <v>125</v>
+      </c>
+      <c r="C128" s="1">
+        <v>1</v>
+      </c>
+      <c r="D128" s="1">
+        <v>2</v>
+      </c>
+      <c r="E128" s="1">
+        <v>200</v>
+      </c>
+      <c r="F128" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="1">
+        <v>10126</v>
+      </c>
+      <c r="B129" s="1">
+        <v>126</v>
+      </c>
+      <c r="C129" s="1">
+        <v>2</v>
+      </c>
+      <c r="D129" s="1">
+        <v>3</v>
+      </c>
+      <c r="E129" s="1">
+        <v>600</v>
+      </c>
+      <c r="F129" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" s="1">
+        <v>10127</v>
+      </c>
+      <c r="B130" s="1">
+        <v>127</v>
+      </c>
+      <c r="C130" s="1">
+        <v>1</v>
+      </c>
+      <c r="D130" s="1">
+        <v>1</v>
+      </c>
+      <c r="E130" s="1">
+        <v>200</v>
+      </c>
+      <c r="F130" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" s="1">
+        <v>10128</v>
+      </c>
+      <c r="B131" s="1">
+        <v>128</v>
+      </c>
+      <c r="C131" s="1">
+        <v>2</v>
+      </c>
+      <c r="D131" s="1">
+        <v>2</v>
+      </c>
+      <c r="E131" s="1">
+        <v>600</v>
+      </c>
+      <c r="F131" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="1">
+        <v>10129</v>
+      </c>
+      <c r="B132" s="1">
+        <v>129</v>
+      </c>
+      <c r="C132" s="1">
+        <v>1</v>
+      </c>
+      <c r="D132" s="1">
+        <v>1</v>
+      </c>
+      <c r="E132" s="1">
+        <v>600</v>
+      </c>
+      <c r="F132" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="1">
+        <v>10130</v>
+      </c>
+      <c r="B133" s="1">
+        <v>130</v>
+      </c>
+      <c r="C133" s="1">
+        <v>2</v>
+      </c>
+      <c r="D133" s="1">
+        <v>2</v>
+      </c>
+      <c r="E133" s="1">
+        <v>200</v>
+      </c>
+      <c r="F133" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+      <c r="C134" s="1"/>
+      <c r="E134" s="1"/>
+      <c r="F134" s="1"/>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="E135" s="1"/>
+      <c r="F135" s="1"/>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="E136" s="1"/>
+      <c r="F136" s="1"/>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="E137" s="1"/>
+      <c r="F137" s="1"/>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="E138" s="1"/>
+      <c r="F138" s="1"/>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="E139" s="1"/>
+      <c r="F139" s="1"/>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="E140" s="1"/>
+      <c r="F140" s="1"/>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="E141" s="1"/>
+      <c r="F141" s="1"/>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="E142" s="1"/>
+      <c r="F142" s="1"/>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="E143" s="1"/>
+      <c r="F143" s="1"/>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="E144" s="1"/>
+    </row>
+    <row r="145" spans="5:5">
+      <c r="E145" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5241,10 +8007,10 @@
       <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -5267,7 +8033,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.5" thickBot="1">
+    <row r="2" spans="1:6" ht="17.25" thickBot="1">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5307,7 +8073,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.5" thickBot="1">
+    <row r="4" spans="1:6" ht="17.25" thickBot="1">
       <c r="A4" s="16">
         <v>7001</v>
       </c>
@@ -5327,7 +8093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.5" thickBot="1">
+    <row r="5" spans="1:6" ht="17.25" thickBot="1">
       <c r="A5" s="16">
         <v>7002</v>
       </c>
@@ -5347,7 +8113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.5" thickBot="1">
+    <row r="6" spans="1:6" ht="17.25" thickBot="1">
       <c r="A6" s="16">
         <v>7003</v>
       </c>
@@ -5367,7 +8133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.5" thickBot="1">
+    <row r="7" spans="1:6" ht="17.25" thickBot="1">
       <c r="A7" s="16">
         <v>7004</v>
       </c>
@@ -5387,7 +8153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.5" thickBot="1">
+    <row r="8" spans="1:6" ht="17.25" thickBot="1">
       <c r="A8" s="16">
         <v>7005</v>
       </c>
@@ -5407,7 +8173,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.5" thickBot="1">
+    <row r="9" spans="1:6" ht="17.25" thickBot="1">
       <c r="A9" s="16">
         <v>7006</v>
       </c>
@@ -5427,7 +8193,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.5" thickBot="1">
+    <row r="10" spans="1:6" ht="17.25" thickBot="1">
       <c r="A10" s="16">
         <v>7007</v>
       </c>
@@ -5447,7 +8213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17.5" thickBot="1">
+    <row r="11" spans="1:6" ht="17.25" thickBot="1">
       <c r="A11" s="16">
         <v>7008</v>
       </c>
@@ -5467,7 +8233,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17.5" thickBot="1">
+    <row r="12" spans="1:6" ht="17.25" thickBot="1">
       <c r="A12" s="16">
         <v>7009</v>
       </c>
@@ -5487,7 +8253,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.5" thickBot="1">
+    <row r="13" spans="1:6" ht="17.25" thickBot="1">
       <c r="A13" s="16">
         <v>7010</v>
       </c>
@@ -5507,7 +8273,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17.5" thickBot="1">
+    <row r="14" spans="1:6" ht="17.25" thickBot="1">
       <c r="A14" s="16">
         <v>7011</v>
       </c>
@@ -5527,7 +8293,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17.5" thickBot="1">
+    <row r="15" spans="1:6" ht="17.25" thickBot="1">
       <c r="A15" s="16">
         <v>7012</v>
       </c>
@@ -5547,7 +8313,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17.5" thickBot="1">
+    <row r="16" spans="1:6" ht="17.25" thickBot="1">
       <c r="A16" s="16">
         <v>7013</v>
       </c>
@@ -5567,7 +8333,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="17.5" thickBot="1">
+    <row r="17" spans="1:6" ht="17.25" thickBot="1">
       <c r="A17" s="16">
         <v>7014</v>
       </c>
@@ -5587,7 +8353,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17.5" thickBot="1">
+    <row r="18" spans="1:6" ht="17.25" thickBot="1">
       <c r="A18" s="16">
         <v>7015</v>
       </c>
@@ -5607,7 +8373,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17.5" thickBot="1">
+    <row r="19" spans="1:6" ht="17.25" thickBot="1">
       <c r="A19" s="16">
         <v>7016</v>
       </c>
@@ -5627,7 +8393,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17.5" thickBot="1">
+    <row r="20" spans="1:6" ht="17.25" thickBot="1">
       <c r="A20" s="16">
         <v>7017</v>
       </c>
@@ -5647,7 +8413,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="17.5" thickBot="1">
+    <row r="21" spans="1:6" ht="17.25" thickBot="1">
       <c r="A21" s="16">
         <v>7018</v>
       </c>
@@ -5667,7 +8433,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17.5" thickBot="1">
+    <row r="22" spans="1:6" ht="17.25" thickBot="1">
       <c r="A22" s="16">
         <v>7019</v>
       </c>
@@ -5687,7 +8453,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="17.5" thickBot="1">
+    <row r="23" spans="1:6" ht="17.25" thickBot="1">
       <c r="A23" s="16">
         <v>7020</v>
       </c>
@@ -5707,7 +8473,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="17.5" thickBot="1">
+    <row r="24" spans="1:6" ht="17.25" thickBot="1">
       <c r="A24" s="16">
         <v>7021</v>
       </c>
@@ -5727,7 +8493,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="17.5" thickBot="1">
+    <row r="25" spans="1:6" ht="17.25" thickBot="1">
       <c r="A25" s="16">
         <v>7022</v>
       </c>
@@ -5747,7 +8513,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="17.5" thickBot="1">
+    <row r="26" spans="1:6" ht="17.25" thickBot="1">
       <c r="A26" s="16">
         <v>7023</v>
       </c>
@@ -5767,7 +8533,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="17.5" thickBot="1">
+    <row r="27" spans="1:6" ht="17.25" thickBot="1">
       <c r="A27" s="16">
         <v>7024</v>
       </c>
@@ -5787,7 +8553,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="17.5" thickBot="1">
+    <row r="28" spans="1:6" ht="17.25" thickBot="1">
       <c r="A28" s="16">
         <v>7025</v>
       </c>
@@ -5807,7 +8573,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="17.5" thickBot="1">
+    <row r="29" spans="1:6" ht="17.25" thickBot="1">
       <c r="A29" s="16">
         <v>7026</v>
       </c>
@@ -5827,7 +8593,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="17.5" thickBot="1">
+    <row r="30" spans="1:6" ht="17.25" thickBot="1">
       <c r="A30" s="16">
         <v>7027</v>
       </c>
@@ -5847,7 +8613,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="17.5" thickBot="1">
+    <row r="31" spans="1:6" ht="17.25" thickBot="1">
       <c r="A31" s="16">
         <v>7028</v>
       </c>
@@ -5867,7 +8633,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="17.5" thickBot="1">
+    <row r="32" spans="1:6" ht="17.25" thickBot="1">
       <c r="A32" s="16">
         <v>7029</v>
       </c>
@@ -5887,7 +8653,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="17.5" thickBot="1">
+    <row r="33" spans="1:6" ht="17.25" thickBot="1">
       <c r="A33" s="16">
         <v>7030</v>
       </c>
@@ -5907,7 +8673,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="17.5" thickBot="1">
+    <row r="34" spans="1:6" ht="17.25" thickBot="1">
       <c r="A34" s="16">
         <v>7031</v>
       </c>
@@ -5927,7 +8693,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="17.5" thickBot="1">
+    <row r="35" spans="1:6" ht="17.25" thickBot="1">
       <c r="A35" s="16">
         <v>7032</v>
       </c>
@@ -5947,7 +8713,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="17.5" thickBot="1">
+    <row r="36" spans="1:6" ht="17.25" thickBot="1">
       <c r="A36" s="16">
         <v>7033</v>
       </c>
@@ -5967,7 +8733,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="17.5" thickBot="1">
+    <row r="37" spans="1:6" ht="17.25" thickBot="1">
       <c r="A37" s="16">
         <v>7034</v>
       </c>
@@ -5987,7 +8753,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="17.5" thickBot="1">
+    <row r="38" spans="1:6" ht="17.25" thickBot="1">
       <c r="A38" s="16">
         <v>7035</v>
       </c>
@@ -6007,7 +8773,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="17.5" thickBot="1">
+    <row r="39" spans="1:6" ht="17.25" thickBot="1">
       <c r="A39" s="16">
         <v>7036</v>
       </c>
@@ -6027,7 +8793,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="17.5" thickBot="1">
+    <row r="40" spans="1:6" ht="17.25" thickBot="1">
       <c r="A40" s="16">
         <v>7037</v>
       </c>
@@ -6047,7 +8813,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="17.5" thickBot="1">
+    <row r="41" spans="1:6" ht="17.25" thickBot="1">
       <c r="A41" s="16">
         <v>7038</v>
       </c>
@@ -6067,7 +8833,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="17.5" thickBot="1">
+    <row r="42" spans="1:6" ht="17.25" thickBot="1">
       <c r="A42" s="16">
         <v>7039</v>
       </c>
@@ -6087,7 +8853,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="17.5" thickBot="1">
+    <row r="43" spans="1:6" ht="17.25" thickBot="1">
       <c r="A43" s="16">
         <v>7040</v>
       </c>
@@ -6107,7 +8873,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="17.5" thickBot="1">
+    <row r="44" spans="1:6" ht="17.25" thickBot="1">
       <c r="A44" s="16">
         <v>7041</v>
       </c>
@@ -6127,7 +8893,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="17.5" thickBot="1">
+    <row r="45" spans="1:6" ht="17.25" thickBot="1">
       <c r="A45" s="16">
         <v>7042</v>
       </c>
@@ -6147,7 +8913,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="17.5" thickBot="1">
+    <row r="46" spans="1:6" ht="17.25" thickBot="1">
       <c r="A46" s="16">
         <v>7043</v>
       </c>
@@ -6167,7 +8933,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="17.5" thickBot="1">
+    <row r="47" spans="1:6" ht="17.25" thickBot="1">
       <c r="A47" s="16">
         <v>7044</v>
       </c>
@@ -6187,7 +8953,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="17.5" thickBot="1">
+    <row r="48" spans="1:6" ht="17.25" thickBot="1">
       <c r="A48" s="16">
         <v>7045</v>
       </c>
@@ -6207,7 +8973,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="17.5" thickBot="1">
+    <row r="49" spans="1:6" ht="17.25" thickBot="1">
       <c r="A49" s="16">
         <v>7046</v>
       </c>
@@ -6227,7 +8993,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="17.5" thickBot="1">
+    <row r="50" spans="1:6" ht="17.25" thickBot="1">
       <c r="A50" s="16">
         <v>7047</v>
       </c>
@@ -6247,7 +9013,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="17.5" thickBot="1">
+    <row r="51" spans="1:6" ht="17.25" thickBot="1">
       <c r="A51" s="16">
         <v>7048</v>
       </c>
@@ -6267,7 +9033,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="17.5" thickBot="1">
+    <row r="52" spans="1:6" ht="17.25" thickBot="1">
       <c r="A52" s="16">
         <v>7049</v>
       </c>
@@ -6287,7 +9053,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="17.5" thickBot="1">
+    <row r="53" spans="1:6" ht="17.25" thickBot="1">
       <c r="A53" s="16">
         <v>7050</v>
       </c>
@@ -6307,7 +9073,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="17.5" thickBot="1">
+    <row r="54" spans="1:6" ht="17.25" thickBot="1">
       <c r="A54" s="14">
         <v>7051</v>
       </c>
@@ -6327,7 +9093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="17.5" thickBot="1">
+    <row r="55" spans="1:6" ht="17.25" thickBot="1">
       <c r="A55" s="16">
         <v>7052</v>
       </c>
@@ -6347,7 +9113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="17.5" thickBot="1">
+    <row r="56" spans="1:6" ht="17.25" thickBot="1">
       <c r="A56" s="16">
         <v>7053</v>
       </c>
@@ -6367,7 +9133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="17.5" thickBot="1">
+    <row r="57" spans="1:6" ht="17.25" thickBot="1">
       <c r="A57" s="16">
         <v>7054</v>
       </c>
@@ -6387,7 +9153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="17.5" thickBot="1">
+    <row r="58" spans="1:6" ht="17.25" thickBot="1">
       <c r="A58" s="16">
         <v>7055</v>
       </c>
@@ -6407,7 +9173,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="17.5" thickBot="1">
+    <row r="59" spans="1:6" ht="17.25" thickBot="1">
       <c r="A59" s="16">
         <v>7056</v>
       </c>
@@ -6427,7 +9193,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="17.5" thickBot="1">
+    <row r="60" spans="1:6" ht="17.25" thickBot="1">
       <c r="A60" s="16">
         <v>7057</v>
       </c>
@@ -6447,7 +9213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="17.5" thickBot="1">
+    <row r="61" spans="1:6" ht="17.25" thickBot="1">
       <c r="A61" s="16">
         <v>7058</v>
       </c>
@@ -6467,7 +9233,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="17.5" thickBot="1">
+    <row r="62" spans="1:6" ht="17.25" thickBot="1">
       <c r="A62" s="16">
         <v>7059</v>
       </c>
@@ -6487,7 +9253,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="17.5" thickBot="1">
+    <row r="63" spans="1:6" ht="17.25" thickBot="1">
       <c r="A63" s="16">
         <v>7060</v>
       </c>
@@ -6507,7 +9273,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="17.5" thickBot="1">
+    <row r="64" spans="1:6" ht="17.25" thickBot="1">
       <c r="A64" s="16">
         <v>7061</v>
       </c>
@@ -6527,7 +9293,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="17.5" thickBot="1">
+    <row r="65" spans="1:6" ht="17.25" thickBot="1">
       <c r="A65" s="16">
         <v>7062</v>
       </c>
@@ -6547,7 +9313,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="17.5" thickBot="1">
+    <row r="66" spans="1:6" ht="17.25" thickBot="1">
       <c r="A66" s="16">
         <v>7063</v>
       </c>
@@ -6567,7 +9333,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="17.5" thickBot="1">
+    <row r="67" spans="1:6" ht="17.25" thickBot="1">
       <c r="A67" s="16">
         <v>7064</v>
       </c>
@@ -6587,7 +9353,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="17.5" thickBot="1">
+    <row r="68" spans="1:6" ht="17.25" thickBot="1">
       <c r="A68" s="16">
         <v>7065</v>
       </c>
@@ -6607,7 +9373,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="17.5" thickBot="1">
+    <row r="69" spans="1:6" ht="17.25" thickBot="1">
       <c r="A69" s="16">
         <v>7066</v>
       </c>
@@ -6627,7 +9393,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="17.5" thickBot="1">
+    <row r="70" spans="1:6" ht="17.25" thickBot="1">
       <c r="A70" s="16">
         <v>7067</v>
       </c>
@@ -6647,7 +9413,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="17.5" thickBot="1">
+    <row r="71" spans="1:6" ht="17.25" thickBot="1">
       <c r="A71" s="16">
         <v>7068</v>
       </c>
@@ -6667,7 +9433,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="17.5" thickBot="1">
+    <row r="72" spans="1:6" ht="17.25" thickBot="1">
       <c r="A72" s="16">
         <v>7069</v>
       </c>
@@ -6687,7 +9453,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="17.5" thickBot="1">
+    <row r="73" spans="1:6" ht="17.25" thickBot="1">
       <c r="A73" s="16">
         <v>7070</v>
       </c>
@@ -6707,7 +9473,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="17.5" thickBot="1">
+    <row r="74" spans="1:6" ht="17.25" thickBot="1">
       <c r="A74" s="16">
         <v>7071</v>
       </c>
@@ -6727,7 +9493,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="17.5" thickBot="1">
+    <row r="75" spans="1:6" ht="17.25" thickBot="1">
       <c r="A75" s="16">
         <v>7072</v>
       </c>
@@ -6747,7 +9513,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="17.5" thickBot="1">
+    <row r="76" spans="1:6" ht="17.25" thickBot="1">
       <c r="A76" s="16">
         <v>7073</v>
       </c>
@@ -6767,7 +9533,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="17.5" thickBot="1">
+    <row r="77" spans="1:6" ht="17.25" thickBot="1">
       <c r="A77" s="16">
         <v>7074</v>
       </c>
@@ -6787,7 +9553,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="17.5" thickBot="1">
+    <row r="78" spans="1:6" ht="17.25" thickBot="1">
       <c r="A78" s="16">
         <v>7075</v>
       </c>
@@ -6807,7 +9573,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="17.5" thickBot="1">
+    <row r="79" spans="1:6" ht="17.25" thickBot="1">
       <c r="A79" s="16">
         <v>7076</v>
       </c>
@@ -6827,7 +9593,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="17.5" thickBot="1">
+    <row r="80" spans="1:6" ht="17.25" thickBot="1">
       <c r="A80" s="16">
         <v>7077</v>
       </c>
@@ -6847,7 +9613,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="17.5" thickBot="1">
+    <row r="81" spans="1:6" ht="17.25" thickBot="1">
       <c r="A81" s="16">
         <v>7078</v>
       </c>
@@ -6867,7 +9633,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="17.5" thickBot="1">
+    <row r="82" spans="1:6" ht="17.25" thickBot="1">
       <c r="A82" s="16">
         <v>7079</v>
       </c>
@@ -6887,7 +9653,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="17.5" thickBot="1">
+    <row r="83" spans="1:6" ht="17.25" thickBot="1">
       <c r="A83" s="16">
         <v>7080</v>
       </c>
@@ -6907,7 +9673,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="17.5" thickBot="1">
+    <row r="84" spans="1:6" ht="17.25" thickBot="1">
       <c r="A84" s="16">
         <v>7081</v>
       </c>
@@ -6927,7 +9693,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="17.5" thickBot="1">
+    <row r="85" spans="1:6" ht="17.25" thickBot="1">
       <c r="A85" s="16">
         <v>7082</v>
       </c>
@@ -6947,7 +9713,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="17.5" thickBot="1">
+    <row r="86" spans="1:6" ht="17.25" thickBot="1">
       <c r="A86" s="16">
         <v>7083</v>
       </c>
@@ -6967,7 +9733,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="17.5" thickBot="1">
+    <row r="87" spans="1:6" ht="17.25" thickBot="1">
       <c r="A87" s="16">
         <v>7084</v>
       </c>
@@ -6987,7 +9753,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="17.5" thickBot="1">
+    <row r="88" spans="1:6" ht="17.25" thickBot="1">
       <c r="A88" s="16">
         <v>7085</v>
       </c>
@@ -7007,7 +9773,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="17.5" thickBot="1">
+    <row r="89" spans="1:6" ht="17.25" thickBot="1">
       <c r="A89" s="16">
         <v>7086</v>
       </c>
@@ -7027,7 +9793,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="17.5" thickBot="1">
+    <row r="90" spans="1:6" ht="17.25" thickBot="1">
       <c r="A90" s="16">
         <v>7087</v>
       </c>
@@ -7047,7 +9813,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="17.5" thickBot="1">
+    <row r="91" spans="1:6" ht="17.25" thickBot="1">
       <c r="A91" s="16">
         <v>7088</v>
       </c>
@@ -7067,7 +9833,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="17.5" thickBot="1">
+    <row r="92" spans="1:6" ht="17.25" thickBot="1">
       <c r="A92" s="16">
         <v>7089</v>
       </c>
@@ -7087,7 +9853,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="17.5" thickBot="1">
+    <row r="93" spans="1:6" ht="17.25" thickBot="1">
       <c r="A93" s="16">
         <v>7090</v>
       </c>
@@ -7107,7 +9873,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="17.5" thickBot="1">
+    <row r="94" spans="1:6" ht="17.25" thickBot="1">
       <c r="A94" s="16">
         <v>7091</v>
       </c>
@@ -7127,7 +9893,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="17.5" thickBot="1">
+    <row r="95" spans="1:6" ht="17.25" thickBot="1">
       <c r="A95" s="16">
         <v>7092</v>
       </c>
@@ -7147,7 +9913,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="17.5" thickBot="1">
+    <row r="96" spans="1:6" ht="17.25" thickBot="1">
       <c r="A96" s="16">
         <v>7093</v>
       </c>
@@ -7167,7 +9933,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="17.5" thickBot="1">
+    <row r="97" spans="1:6" ht="17.25" thickBot="1">
       <c r="A97" s="16">
         <v>7094</v>
       </c>
@@ -7187,7 +9953,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="17.5" thickBot="1">
+    <row r="98" spans="1:6" ht="17.25" thickBot="1">
       <c r="A98" s="16">
         <v>7095</v>
       </c>
@@ -7207,7 +9973,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="17.5" thickBot="1">
+    <row r="99" spans="1:6" ht="17.25" thickBot="1">
       <c r="A99" s="16">
         <v>7096</v>
       </c>
@@ -7227,7 +9993,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="17.5" thickBot="1">
+    <row r="100" spans="1:6" ht="17.25" thickBot="1">
       <c r="A100" s="16">
         <v>7097</v>
       </c>
@@ -7247,7 +10013,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="17.5" thickBot="1">
+    <row r="101" spans="1:6" ht="17.25" thickBot="1">
       <c r="A101" s="16">
         <v>7098</v>
       </c>
@@ -7267,7 +10033,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="17.5" thickBot="1">
+    <row r="102" spans="1:6" ht="17.25" thickBot="1">
       <c r="A102" s="16">
         <v>7099</v>
       </c>
@@ -7287,7 +10053,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="17.5" thickBot="1">
+    <row r="103" spans="1:6" ht="17.25" thickBot="1">
       <c r="A103" s="16">
         <v>7100</v>
       </c>
@@ -7322,10 +10088,10 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="104.83203125" customWidth="1"/>
-    <col min="3" max="3" width="7.08203125" customWidth="1"/>
+    <col min="2" max="2" width="104.875" customWidth="1"/>
+    <col min="3" max="3" width="7.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -7372,7 +10138,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="51">
+    <row r="5" spans="1:3" ht="49.5">
       <c r="A5">
         <v>1</v>
       </c>
@@ -7383,7 +10149,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="85">
+    <row r="6" spans="1:3" ht="82.5">
       <c r="A6">
         <v>2</v>
       </c>
@@ -7394,7 +10160,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="85">
+    <row r="7" spans="1:3" ht="82.5">
       <c r="A7">
         <v>3</v>
       </c>
@@ -7405,7 +10171,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51">
+    <row r="8" spans="1:3" ht="49.5">
       <c r="A8">
         <v>4</v>
       </c>
@@ -7416,7 +10182,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="85">
+    <row r="9" spans="1:3" ht="82.5">
       <c r="A9">
         <v>5</v>
       </c>
@@ -7427,7 +10193,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="68">
+    <row r="10" spans="1:3" ht="66">
       <c r="A10">
         <v>6</v>
       </c>
@@ -7438,7 +10204,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="51">
+    <row r="11" spans="1:3" ht="49.5">
       <c r="A11">
         <v>7</v>
       </c>
@@ -7449,7 +10215,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="68">
+    <row r="12" spans="1:3" ht="66">
       <c r="A12">
         <v>8</v>
       </c>
@@ -7460,7 +10226,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="34">
+    <row r="13" spans="1:3" ht="33">
       <c r="A13">
         <v>9</v>
       </c>
@@ -7471,7 +10237,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="119">
+    <row r="14" spans="1:3" ht="115.5">
       <c r="A14">
         <v>10</v>
       </c>
@@ -7482,7 +10248,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="85">
+    <row r="15" spans="1:3" ht="82.5">
       <c r="A15">
         <v>11</v>
       </c>
@@ -7519,14 +10285,14 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="8.58203125" customWidth="1"/>
-    <col min="3" max="3" width="22.58203125" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.08203125" customWidth="1"/>
+    <col min="1" max="1" width="8.625" customWidth="1"/>
+    <col min="3" max="3" width="22.625" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
+    <col min="5" max="5" width="20.125" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -7575,7 +10341,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17.5" thickBot="1">
+    <row r="3" spans="1:7" ht="17.25" thickBot="1">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -7598,7 +10364,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17.5" thickBot="1">
+    <row r="4" spans="1:7" ht="17.25" thickBot="1">
       <c r="A4" s="14">
         <v>401</v>
       </c>
@@ -7621,7 +10387,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.5" thickBot="1">
+    <row r="5" spans="1:7" ht="17.25" thickBot="1">
       <c r="A5" s="16">
         <v>402</v>
       </c>
@@ -7644,7 +10410,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17.5" thickBot="1">
+    <row r="6" spans="1:7" ht="17.25" thickBot="1">
       <c r="A6" s="16">
         <v>403</v>
       </c>
@@ -7667,7 +10433,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17.5" thickBot="1">
+    <row r="7" spans="1:7" ht="17.25" thickBot="1">
       <c r="A7" s="16">
         <v>404</v>
       </c>
@@ -7690,7 +10456,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17.5" thickBot="1">
+    <row r="8" spans="1:7" ht="17.25" thickBot="1">
       <c r="A8" s="16">
         <v>405</v>
       </c>
@@ -7713,7 +10479,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17.5" thickBot="1">
+    <row r="9" spans="1:7" ht="17.25" thickBot="1">
       <c r="A9" s="16">
         <v>406</v>
       </c>
@@ -7736,7 +10502,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.5" thickBot="1">
+    <row r="10" spans="1:7" ht="17.25" thickBot="1">
       <c r="A10" s="16">
         <v>407</v>
       </c>
@@ -7759,7 +10525,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17.5" thickBot="1">
+    <row r="11" spans="1:7" ht="17.25" thickBot="1">
       <c r="A11" s="16">
         <v>408</v>
       </c>
@@ -7782,7 +10548,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.5" thickBot="1">
+    <row r="12" spans="1:7" ht="17.25" thickBot="1">
       <c r="A12" s="16">
         <v>409</v>
       </c>
@@ -7805,7 +10571,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17.5" thickBot="1">
+    <row r="13" spans="1:7" ht="17.25" thickBot="1">
       <c r="A13" s="16">
         <v>410</v>
       </c>
@@ -7843,13 +10609,13 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.58203125" customWidth="1"/>
-    <col min="6" max="6" width="13.58203125" customWidth="1"/>
-    <col min="7" max="7" width="19.08203125" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
+    <col min="5" max="5" width="20.625" customWidth="1"/>
+    <col min="6" max="6" width="13.625" customWidth="1"/>
+    <col min="7" max="7" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -7898,7 +10664,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17.5" thickBot="1">
+    <row r="3" spans="1:7" ht="17.25" thickBot="1">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -7921,7 +10687,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17.5" thickBot="1">
+    <row r="4" spans="1:7" ht="17.25" thickBot="1">
       <c r="A4" s="14">
         <v>501</v>
       </c>
@@ -7944,7 +10710,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.5" thickBot="1">
+    <row r="5" spans="1:7" ht="17.25" thickBot="1">
       <c r="A5" s="16">
         <v>502</v>
       </c>
@@ -7967,7 +10733,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17.5" thickBot="1">
+    <row r="6" spans="1:7" ht="17.25" thickBot="1">
       <c r="A6" s="16">
         <v>503</v>
       </c>
@@ -7990,7 +10756,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17.5" thickBot="1">
+    <row r="7" spans="1:7" ht="17.25" thickBot="1">
       <c r="A7" s="16">
         <v>504</v>
       </c>
@@ -8013,7 +10779,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17.5" thickBot="1">
+    <row r="8" spans="1:7" ht="17.25" thickBot="1">
       <c r="A8" s="16">
         <v>505</v>
       </c>
@@ -8051,21 +10817,21 @@
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="8.58203125" customWidth="1"/>
-    <col min="2" max="2" width="31.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.625" customWidth="1"/>
+    <col min="2" max="2" width="31.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.08203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.58203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.08203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.58203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.58203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.58203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -8209,7 +10975,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="51">
+    <row r="4" spans="1:15" ht="49.5">
       <c r="A4">
         <v>3001</v>
       </c>
@@ -8256,7 +11022,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="51">
+    <row r="5" spans="1:15" ht="49.5">
       <c r="A5">
         <v>3002</v>
       </c>
@@ -8303,7 +11069,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="68">
+    <row r="6" spans="1:15" ht="66">
       <c r="A6">
         <v>3003</v>
       </c>
@@ -8350,7 +11116,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="51">
+    <row r="7" spans="1:15" ht="49.5">
       <c r="A7">
         <v>3004</v>
       </c>
@@ -8397,7 +11163,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="51">
+    <row r="8" spans="1:15" ht="49.5">
       <c r="A8">
         <v>3005</v>
       </c>
@@ -8444,7 +11210,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="51">
+    <row r="9" spans="1:15" ht="49.5">
       <c r="A9">
         <v>3006</v>
       </c>
@@ -8491,7 +11257,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="51">
+    <row r="10" spans="1:15" ht="49.5">
       <c r="A10">
         <v>3007</v>
       </c>
@@ -8538,7 +11304,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="51">
+    <row r="11" spans="1:15" ht="49.5">
       <c r="A11">
         <v>3008</v>
       </c>
@@ -8600,15 +11366,15 @@
       <selection sqref="A1:M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="6.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.08203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.58203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -9610,7 +12376,7 @@
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="37" style="1" customWidth="1"/>
@@ -10260,7 +13026,7 @@
       <selection activeCell="E1" sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">

</xml_diff>